<commit_message>
Clean up before editing the paper
</commit_message>
<xml_diff>
--- a/raw data/20190714_excel tsh2_2019_data.xlsx
+++ b/raw data/20190714_excel tsh2_2019_data.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simontuke/Dropbox/TSH_2019/raw data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F1FDB8-79B2-9F43-A85D-834697430C70}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,25 +18,25 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$S$1:$S$507</definedName>
   </definedNames>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="124519"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nigel Bean</author>
   </authors>
   <commentList>
-    <comment ref="D326" authorId="0">
+    <comment ref="D326" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -68,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6601" uniqueCount="691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7027" uniqueCount="690">
   <si>
     <t>Paper</t>
   </si>
@@ -2160,14 +2166,11 @@
   <si>
     <t>hypo</t>
   </si>
-  <si>
-    <t>hyper(cont)</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7">
     <font>
       <sz val="12"/>
@@ -3371,40 +3374,40 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W507"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="P497" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E471" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T505" sqref="T505"/>
+      <selection pane="bottomRight" activeCell="A518" sqref="A518"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
-    <col min="2" max="2" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.125" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.1640625" customWidth="1"/>
     <col min="4" max="4" width="60.5" customWidth="1"/>
-    <col min="5" max="5" width="19.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.625" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" customWidth="1"/>
     <col min="7" max="7" width="11.5" customWidth="1"/>
-    <col min="8" max="8" width="13.125" customWidth="1"/>
-    <col min="9" max="9" width="16.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" customWidth="1"/>
+    <col min="9" max="9" width="16.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="161.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.5" customWidth="1"/>
-    <col min="14" max="14" width="15.625" customWidth="1"/>
-    <col min="15" max="15" width="13.125" customWidth="1"/>
-    <col min="20" max="21" width="19.875" customWidth="1"/>
-    <col min="22" max="22" width="18.125" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" customWidth="1"/>
+    <col min="15" max="15" width="13.1640625" customWidth="1"/>
+    <col min="20" max="21" width="19.83203125" customWidth="1"/>
+    <col min="22" max="22" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -3550,6 +3553,9 @@
       </c>
     </row>
     <row r="3" spans="1:23">
+      <c r="A3" t="s">
+        <v>688</v>
+      </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -3618,6 +3624,9 @@
       </c>
     </row>
     <row r="4" spans="1:23">
+      <c r="A4" t="s">
+        <v>688</v>
+      </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -3686,6 +3695,9 @@
       </c>
     </row>
     <row r="5" spans="1:23">
+      <c r="A5" t="s">
+        <v>688</v>
+      </c>
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -3754,6 +3766,9 @@
       </c>
     </row>
     <row r="6" spans="1:23">
+      <c r="A6" t="s">
+        <v>688</v>
+      </c>
       <c r="B6" t="s">
         <v>1</v>
       </c>
@@ -3822,6 +3837,9 @@
       </c>
     </row>
     <row r="7" spans="1:23">
+      <c r="A7" t="s">
+        <v>688</v>
+      </c>
       <c r="B7" t="s">
         <v>1</v>
       </c>
@@ -3890,6 +3908,9 @@
       </c>
     </row>
     <row r="8" spans="1:23">
+      <c r="A8" t="s">
+        <v>688</v>
+      </c>
       <c r="B8" t="s">
         <v>1</v>
       </c>
@@ -3958,6 +3979,9 @@
       </c>
     </row>
     <row r="9" spans="1:23">
+      <c r="A9" t="s">
+        <v>688</v>
+      </c>
       <c r="B9" t="s">
         <v>1</v>
       </c>
@@ -4026,6 +4050,9 @@
       </c>
     </row>
     <row r="10" spans="1:23">
+      <c r="A10" t="s">
+        <v>688</v>
+      </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
@@ -4094,6 +4121,9 @@
       </c>
     </row>
     <row r="11" spans="1:23">
+      <c r="A11" t="s">
+        <v>688</v>
+      </c>
       <c r="B11" t="s">
         <v>1</v>
       </c>
@@ -4162,6 +4192,9 @@
       </c>
     </row>
     <row r="12" spans="1:23">
+      <c r="A12" t="s">
+        <v>688</v>
+      </c>
       <c r="B12" t="s">
         <v>1</v>
       </c>
@@ -4230,6 +4263,9 @@
       </c>
     </row>
     <row r="13" spans="1:23">
+      <c r="A13" t="s">
+        <v>688</v>
+      </c>
       <c r="B13" t="s">
         <v>1</v>
       </c>
@@ -4298,6 +4334,9 @@
       </c>
     </row>
     <row r="14" spans="1:23">
+      <c r="A14" t="s">
+        <v>688</v>
+      </c>
       <c r="B14" t="s">
         <v>1</v>
       </c>
@@ -4366,6 +4405,9 @@
       </c>
     </row>
     <row r="15" spans="1:23">
+      <c r="A15" t="s">
+        <v>688</v>
+      </c>
       <c r="B15" t="s">
         <v>1</v>
       </c>
@@ -4434,6 +4476,9 @@
       </c>
     </row>
     <row r="17" spans="1:16">
+      <c r="A17" t="s">
+        <v>688</v>
+      </c>
       <c r="B17" t="s">
         <v>1</v>
       </c>
@@ -4481,6 +4526,9 @@
       </c>
     </row>
     <row r="18" spans="1:16">
+      <c r="A18" t="s">
+        <v>688</v>
+      </c>
       <c r="B18" t="s">
         <v>1</v>
       </c>
@@ -4528,6 +4576,9 @@
       </c>
     </row>
     <row r="19" spans="1:16">
+      <c r="A19" t="s">
+        <v>688</v>
+      </c>
       <c r="B19" t="s">
         <v>1</v>
       </c>
@@ -4575,6 +4626,9 @@
       </c>
     </row>
     <row r="20" spans="1:16">
+      <c r="A20" t="s">
+        <v>688</v>
+      </c>
       <c r="B20" t="s">
         <v>1</v>
       </c>
@@ -4622,6 +4676,9 @@
       </c>
     </row>
     <row r="21" spans="1:16">
+      <c r="A21" t="s">
+        <v>688</v>
+      </c>
       <c r="B21" t="s">
         <v>1</v>
       </c>
@@ -4669,6 +4726,9 @@
       </c>
     </row>
     <row r="22" spans="1:16">
+      <c r="A22" t="s">
+        <v>688</v>
+      </c>
       <c r="B22" t="s">
         <v>1</v>
       </c>
@@ -4766,6 +4826,9 @@
       </c>
     </row>
     <row r="25" spans="1:16">
+      <c r="A25" t="s">
+        <v>688</v>
+      </c>
       <c r="B25" t="s">
         <v>48</v>
       </c>
@@ -4813,6 +4876,9 @@
       </c>
     </row>
     <row r="26" spans="1:16">
+      <c r="A26" t="s">
+        <v>688</v>
+      </c>
       <c r="B26" t="s">
         <v>48</v>
       </c>
@@ -4860,6 +4926,9 @@
       </c>
     </row>
     <row r="27" spans="1:16">
+      <c r="A27" t="s">
+        <v>688</v>
+      </c>
       <c r="B27" t="s">
         <v>48</v>
       </c>
@@ -4904,6 +4973,9 @@
       </c>
     </row>
     <row r="28" spans="1:16">
+      <c r="A28" t="s">
+        <v>688</v>
+      </c>
       <c r="B28" t="s">
         <v>48</v>
       </c>
@@ -4951,6 +5023,9 @@
       </c>
     </row>
     <row r="29" spans="1:16">
+      <c r="A29" t="s">
+        <v>688</v>
+      </c>
       <c r="B29" t="s">
         <v>48</v>
       </c>
@@ -4995,6 +5070,9 @@
       </c>
     </row>
     <row r="31" spans="1:16">
+      <c r="A31" t="s">
+        <v>688</v>
+      </c>
       <c r="B31" t="s">
         <v>499</v>
       </c>
@@ -5042,6 +5120,9 @@
       </c>
     </row>
     <row r="32" spans="1:16">
+      <c r="A32" t="s">
+        <v>688</v>
+      </c>
       <c r="B32" t="s">
         <v>499</v>
       </c>
@@ -5086,6 +5167,9 @@
       </c>
     </row>
     <row r="33" spans="1:16">
+      <c r="A33" t="s">
+        <v>688</v>
+      </c>
       <c r="B33" t="s">
         <v>499</v>
       </c>
@@ -5133,6 +5217,9 @@
       </c>
     </row>
     <row r="34" spans="1:16">
+      <c r="A34" t="s">
+        <v>688</v>
+      </c>
       <c r="B34" t="s">
         <v>499</v>
       </c>
@@ -5180,6 +5267,9 @@
       </c>
     </row>
     <row r="35" spans="1:16">
+      <c r="A35" t="s">
+        <v>688</v>
+      </c>
       <c r="B35" t="s">
         <v>499</v>
       </c>
@@ -5227,6 +5317,9 @@
       </c>
     </row>
     <row r="36" spans="1:16">
+      <c r="A36" t="s">
+        <v>688</v>
+      </c>
       <c r="B36" t="s">
         <v>499</v>
       </c>
@@ -5324,6 +5417,9 @@
       </c>
     </row>
     <row r="39" spans="1:16">
+      <c r="A39" t="s">
+        <v>688</v>
+      </c>
       <c r="B39" t="s">
         <v>70</v>
       </c>
@@ -5371,6 +5467,9 @@
       </c>
     </row>
     <row r="40" spans="1:16">
+      <c r="A40" t="s">
+        <v>688</v>
+      </c>
       <c r="B40" t="s">
         <v>70</v>
       </c>
@@ -5418,6 +5517,9 @@
       </c>
     </row>
     <row r="41" spans="1:16">
+      <c r="A41" t="s">
+        <v>688</v>
+      </c>
       <c r="B41" t="s">
         <v>70</v>
       </c>
@@ -5465,6 +5567,9 @@
       </c>
     </row>
     <row r="42" spans="1:16">
+      <c r="A42" t="s">
+        <v>688</v>
+      </c>
       <c r="B42" t="s">
         <v>70</v>
       </c>
@@ -5512,6 +5617,9 @@
       </c>
     </row>
     <row r="43" spans="1:16">
+      <c r="A43" t="s">
+        <v>688</v>
+      </c>
       <c r="B43" t="s">
         <v>70</v>
       </c>
@@ -5559,6 +5667,9 @@
       </c>
     </row>
     <row r="44" spans="1:16">
+      <c r="A44" t="s">
+        <v>688</v>
+      </c>
       <c r="B44" t="s">
         <v>70</v>
       </c>
@@ -5656,6 +5767,9 @@
       </c>
     </row>
     <row r="47" spans="1:16">
+      <c r="A47" t="s">
+        <v>688</v>
+      </c>
       <c r="B47" t="s">
         <v>501</v>
       </c>
@@ -5753,6 +5867,9 @@
       </c>
     </row>
     <row r="50" spans="1:16">
+      <c r="A50" t="s">
+        <v>688</v>
+      </c>
       <c r="B50" t="s">
         <v>85</v>
       </c>
@@ -5800,6 +5917,9 @@
       </c>
     </row>
     <row r="51" spans="1:16">
+      <c r="A51" t="s">
+        <v>688</v>
+      </c>
       <c r="B51" t="s">
         <v>85</v>
       </c>
@@ -5847,6 +5967,9 @@
       </c>
     </row>
     <row r="52" spans="1:16">
+      <c r="A52" t="s">
+        <v>688</v>
+      </c>
       <c r="B52" t="s">
         <v>85</v>
       </c>
@@ -5894,6 +6017,9 @@
       </c>
     </row>
     <row r="53" spans="1:16">
+      <c r="A53" t="s">
+        <v>688</v>
+      </c>
       <c r="B53" t="s">
         <v>85</v>
       </c>
@@ -5941,6 +6067,9 @@
       </c>
     </row>
     <row r="54" spans="1:16">
+      <c r="A54" t="s">
+        <v>688</v>
+      </c>
       <c r="B54" t="s">
         <v>85</v>
       </c>
@@ -5988,6 +6117,9 @@
       </c>
     </row>
     <row r="55" spans="1:16">
+      <c r="A55" t="s">
+        <v>688</v>
+      </c>
       <c r="B55" t="s">
         <v>85</v>
       </c>
@@ -6035,6 +6167,9 @@
       </c>
     </row>
     <row r="56" spans="1:16">
+      <c r="A56" t="s">
+        <v>688</v>
+      </c>
       <c r="B56" t="s">
         <v>85</v>
       </c>
@@ -6082,6 +6217,9 @@
       </c>
     </row>
     <row r="57" spans="1:16">
+      <c r="A57" t="s">
+        <v>688</v>
+      </c>
       <c r="B57" t="s">
         <v>85</v>
       </c>
@@ -6179,6 +6317,9 @@
       </c>
     </row>
     <row r="62" spans="1:16">
+      <c r="A62" t="s">
+        <v>688</v>
+      </c>
       <c r="B62" t="s">
         <v>103</v>
       </c>
@@ -6226,6 +6367,9 @@
       </c>
     </row>
     <row r="63" spans="1:16">
+      <c r="A63" t="s">
+        <v>688</v>
+      </c>
       <c r="B63" t="s">
         <v>103</v>
       </c>
@@ -6273,6 +6417,9 @@
       </c>
     </row>
     <row r="64" spans="1:16">
+      <c r="A64" t="s">
+        <v>688</v>
+      </c>
       <c r="B64" t="s">
         <v>103</v>
       </c>
@@ -6320,6 +6467,9 @@
       </c>
     </row>
     <row r="65" spans="1:16">
+      <c r="A65" t="s">
+        <v>688</v>
+      </c>
       <c r="B65" t="s">
         <v>103</v>
       </c>
@@ -6367,6 +6517,9 @@
       </c>
     </row>
     <row r="66" spans="1:16">
+      <c r="A66" t="s">
+        <v>688</v>
+      </c>
       <c r="B66" t="s">
         <v>103</v>
       </c>
@@ -6455,6 +6608,9 @@
       </c>
     </row>
     <row r="69" spans="1:16">
+      <c r="A69" t="s">
+        <v>688</v>
+      </c>
       <c r="B69" t="s">
         <v>107</v>
       </c>
@@ -6502,6 +6658,9 @@
       </c>
     </row>
     <row r="70" spans="1:16">
+      <c r="A70" t="s">
+        <v>688</v>
+      </c>
       <c r="B70" t="s">
         <v>107</v>
       </c>
@@ -6549,6 +6708,9 @@
       </c>
     </row>
     <row r="71" spans="1:16">
+      <c r="A71" t="s">
+        <v>688</v>
+      </c>
       <c r="B71" t="s">
         <v>107</v>
       </c>
@@ -6596,6 +6758,9 @@
       </c>
     </row>
     <row r="72" spans="1:16">
+      <c r="A72" t="s">
+        <v>688</v>
+      </c>
       <c r="B72" t="s">
         <v>107</v>
       </c>
@@ -6643,6 +6808,9 @@
       </c>
     </row>
     <row r="73" spans="1:16">
+      <c r="A73" t="s">
+        <v>688</v>
+      </c>
       <c r="B73" t="s">
         <v>107</v>
       </c>
@@ -6690,6 +6858,9 @@
       </c>
     </row>
     <row r="74" spans="1:16">
+      <c r="A74" t="s">
+        <v>688</v>
+      </c>
       <c r="B74" t="s">
         <v>107</v>
       </c>
@@ -6737,6 +6908,9 @@
       </c>
     </row>
     <row r="75" spans="1:16">
+      <c r="A75" t="s">
+        <v>688</v>
+      </c>
       <c r="B75" t="s">
         <v>107</v>
       </c>
@@ -6784,6 +6958,9 @@
       </c>
     </row>
     <row r="76" spans="1:16">
+      <c r="A76" t="s">
+        <v>688</v>
+      </c>
       <c r="B76" t="s">
         <v>107</v>
       </c>
@@ -6831,6 +7008,9 @@
       </c>
     </row>
     <row r="77" spans="1:16">
+      <c r="A77" t="s">
+        <v>688</v>
+      </c>
       <c r="B77" t="s">
         <v>107</v>
       </c>
@@ -6878,6 +7058,9 @@
       </c>
     </row>
     <row r="78" spans="1:16">
+      <c r="A78" t="s">
+        <v>688</v>
+      </c>
       <c r="B78" t="s">
         <v>107</v>
       </c>
@@ -6925,6 +7108,9 @@
       </c>
     </row>
     <row r="79" spans="1:16">
+      <c r="A79" t="s">
+        <v>688</v>
+      </c>
       <c r="B79" t="s">
         <v>107</v>
       </c>
@@ -6972,6 +7158,9 @@
       </c>
     </row>
     <row r="80" spans="1:16">
+      <c r="A80" t="s">
+        <v>688</v>
+      </c>
       <c r="B80" t="s">
         <v>107</v>
       </c>
@@ -7019,6 +7208,9 @@
       </c>
     </row>
     <row r="81" spans="1:23">
+      <c r="A81" t="s">
+        <v>688</v>
+      </c>
       <c r="B81" t="s">
         <v>107</v>
       </c>
@@ -7140,6 +7332,9 @@
       </c>
     </row>
     <row r="85" spans="1:23">
+      <c r="A85" t="s">
+        <v>688</v>
+      </c>
       <c r="B85" t="s">
         <v>116</v>
       </c>
@@ -7208,6 +7403,9 @@
       </c>
     </row>
     <row r="86" spans="1:23">
+      <c r="A86" t="s">
+        <v>688</v>
+      </c>
       <c r="B86" t="s">
         <v>116</v>
       </c>
@@ -7276,6 +7474,9 @@
       </c>
     </row>
     <row r="87" spans="1:23">
+      <c r="A87" t="s">
+        <v>688</v>
+      </c>
       <c r="B87" t="s">
         <v>116</v>
       </c>
@@ -7344,6 +7545,9 @@
       </c>
     </row>
     <row r="88" spans="1:23">
+      <c r="A88" t="s">
+        <v>688</v>
+      </c>
       <c r="B88" t="s">
         <v>116</v>
       </c>
@@ -7412,6 +7616,9 @@
       </c>
     </row>
     <row r="89" spans="1:23">
+      <c r="A89" t="s">
+        <v>688</v>
+      </c>
       <c r="B89" t="s">
         <v>116</v>
       </c>
@@ -7480,6 +7687,9 @@
       </c>
     </row>
     <row r="90" spans="1:23">
+      <c r="A90" t="s">
+        <v>688</v>
+      </c>
       <c r="B90" t="s">
         <v>116</v>
       </c>
@@ -7548,6 +7758,9 @@
       </c>
     </row>
     <row r="91" spans="1:23">
+      <c r="A91" t="s">
+        <v>688</v>
+      </c>
       <c r="B91" t="s">
         <v>116</v>
       </c>
@@ -7616,6 +7829,9 @@
       </c>
     </row>
     <row r="92" spans="1:23">
+      <c r="A92" t="s">
+        <v>688</v>
+      </c>
       <c r="B92" t="s">
         <v>116</v>
       </c>
@@ -7684,6 +7900,9 @@
       </c>
     </row>
     <row r="93" spans="1:23">
+      <c r="A93" t="s">
+        <v>688</v>
+      </c>
       <c r="B93" t="s">
         <v>116</v>
       </c>
@@ -7752,6 +7971,9 @@
       </c>
     </row>
     <row r="94" spans="1:23">
+      <c r="A94" t="s">
+        <v>688</v>
+      </c>
       <c r="B94" t="s">
         <v>116</v>
       </c>
@@ -7820,6 +8042,9 @@
       </c>
     </row>
     <row r="95" spans="1:23">
+      <c r="A95" t="s">
+        <v>688</v>
+      </c>
       <c r="B95" t="s">
         <v>116</v>
       </c>
@@ -7965,6 +8190,9 @@
       </c>
     </row>
     <row r="99" spans="1:23">
+      <c r="A99" t="s">
+        <v>688</v>
+      </c>
       <c r="B99" t="s">
         <v>130</v>
       </c>
@@ -8033,6 +8261,9 @@
       </c>
     </row>
     <row r="100" spans="1:23">
+      <c r="A100" t="s">
+        <v>688</v>
+      </c>
       <c r="B100" t="s">
         <v>130</v>
       </c>
@@ -8101,6 +8332,9 @@
       </c>
     </row>
     <row r="101" spans="1:23">
+      <c r="A101" t="s">
+        <v>688</v>
+      </c>
       <c r="B101" t="s">
         <v>130</v>
       </c>
@@ -8169,6 +8403,9 @@
       </c>
     </row>
     <row r="102" spans="1:23">
+      <c r="A102" t="s">
+        <v>688</v>
+      </c>
       <c r="B102" t="s">
         <v>130</v>
       </c>
@@ -8237,6 +8474,9 @@
       </c>
     </row>
     <row r="103" spans="1:23">
+      <c r="A103" t="s">
+        <v>688</v>
+      </c>
       <c r="B103" t="s">
         <v>130</v>
       </c>
@@ -8305,6 +8545,9 @@
       </c>
     </row>
     <row r="104" spans="1:23">
+      <c r="A104" t="s">
+        <v>688</v>
+      </c>
       <c r="B104" t="s">
         <v>130</v>
       </c>
@@ -8373,6 +8616,9 @@
       </c>
     </row>
     <row r="105" spans="1:23">
+      <c r="A105" t="s">
+        <v>688</v>
+      </c>
       <c r="B105" t="s">
         <v>130</v>
       </c>
@@ -8441,6 +8687,9 @@
       </c>
     </row>
     <row r="106" spans="1:23">
+      <c r="A106" t="s">
+        <v>688</v>
+      </c>
       <c r="B106" t="s">
         <v>130</v>
       </c>
@@ -8509,6 +8758,9 @@
       </c>
     </row>
     <row r="107" spans="1:23">
+      <c r="A107" t="s">
+        <v>688</v>
+      </c>
       <c r="B107" t="s">
         <v>130</v>
       </c>
@@ -8577,6 +8829,9 @@
       </c>
     </row>
     <row r="108" spans="1:23">
+      <c r="A108" t="s">
+        <v>688</v>
+      </c>
       <c r="B108" t="s">
         <v>130</v>
       </c>
@@ -8645,6 +8900,9 @@
       </c>
     </row>
     <row r="109" spans="1:23">
+      <c r="A109" t="s">
+        <v>688</v>
+      </c>
       <c r="B109" t="s">
         <v>130</v>
       </c>
@@ -8787,6 +9045,9 @@
       </c>
     </row>
     <row r="112" spans="1:23">
+      <c r="A112" t="s">
+        <v>688</v>
+      </c>
       <c r="B112" t="s">
         <v>146</v>
       </c>
@@ -8854,7 +9115,10 @@
         <v>674</v>
       </c>
     </row>
-    <row r="113" spans="2:23">
+    <row r="113" spans="1:23">
+      <c r="A113" t="s">
+        <v>688</v>
+      </c>
       <c r="B113" t="s">
         <v>146</v>
       </c>
@@ -8922,7 +9186,10 @@
         <v>674</v>
       </c>
     </row>
-    <row r="114" spans="2:23">
+    <row r="114" spans="1:23">
+      <c r="A114" t="s">
+        <v>688</v>
+      </c>
       <c r="B114" t="s">
         <v>146</v>
       </c>
@@ -8990,7 +9257,10 @@
         <v>674</v>
       </c>
     </row>
-    <row r="115" spans="2:23">
+    <row r="115" spans="1:23">
+      <c r="A115" t="s">
+        <v>688</v>
+      </c>
       <c r="B115" t="s">
         <v>146</v>
       </c>
@@ -9058,7 +9328,10 @@
         <v>674</v>
       </c>
     </row>
-    <row r="116" spans="2:23">
+    <row r="116" spans="1:23">
+      <c r="A116" t="s">
+        <v>688</v>
+      </c>
       <c r="B116" t="s">
         <v>146</v>
       </c>
@@ -9126,7 +9399,10 @@
         <v>674</v>
       </c>
     </row>
-    <row r="117" spans="2:23">
+    <row r="117" spans="1:23">
+      <c r="A117" t="s">
+        <v>688</v>
+      </c>
       <c r="B117" t="s">
         <v>146</v>
       </c>
@@ -9194,7 +9470,10 @@
         <v>674</v>
       </c>
     </row>
-    <row r="118" spans="2:23">
+    <row r="118" spans="1:23">
+      <c r="A118" t="s">
+        <v>688</v>
+      </c>
       <c r="B118" t="s">
         <v>146</v>
       </c>
@@ -9262,7 +9541,10 @@
         <v>674</v>
       </c>
     </row>
-    <row r="119" spans="2:23">
+    <row r="119" spans="1:23">
+      <c r="A119" t="s">
+        <v>688</v>
+      </c>
       <c r="B119" t="s">
         <v>146</v>
       </c>
@@ -9330,7 +9612,10 @@
         <v>674</v>
       </c>
     </row>
-    <row r="120" spans="2:23">
+    <row r="120" spans="1:23">
+      <c r="A120" t="s">
+        <v>688</v>
+      </c>
       <c r="B120" t="s">
         <v>146</v>
       </c>
@@ -9398,7 +9683,10 @@
         <v>674</v>
       </c>
     </row>
-    <row r="121" spans="2:23">
+    <row r="121" spans="1:23">
+      <c r="A121" t="s">
+        <v>688</v>
+      </c>
       <c r="B121" t="s">
         <v>146</v>
       </c>
@@ -9466,7 +9754,10 @@
         <v>674</v>
       </c>
     </row>
-    <row r="122" spans="2:23">
+    <row r="122" spans="1:23">
+      <c r="A122" t="s">
+        <v>688</v>
+      </c>
       <c r="B122" t="s">
         <v>146</v>
       </c>
@@ -9534,7 +9825,10 @@
         <v>674</v>
       </c>
     </row>
-    <row r="123" spans="2:23">
+    <row r="123" spans="1:23">
+      <c r="A123" t="s">
+        <v>688</v>
+      </c>
       <c r="B123" t="s">
         <v>146</v>
       </c>
@@ -9602,7 +9896,10 @@
         <v>674</v>
       </c>
     </row>
-    <row r="124" spans="2:23">
+    <row r="124" spans="1:23">
+      <c r="A124" t="s">
+        <v>688</v>
+      </c>
       <c r="B124" t="s">
         <v>146</v>
       </c>
@@ -9670,7 +9967,10 @@
         <v>674</v>
       </c>
     </row>
-    <row r="125" spans="2:23">
+    <row r="125" spans="1:23">
+      <c r="A125" t="s">
+        <v>688</v>
+      </c>
       <c r="B125" t="s">
         <v>146</v>
       </c>
@@ -9738,7 +10038,10 @@
         <v>674</v>
       </c>
     </row>
-    <row r="126" spans="2:23">
+    <row r="126" spans="1:23">
+      <c r="A126" t="s">
+        <v>688</v>
+      </c>
       <c r="B126" t="s">
         <v>146</v>
       </c>
@@ -9806,7 +10109,10 @@
         <v>674</v>
       </c>
     </row>
-    <row r="127" spans="2:23">
+    <row r="127" spans="1:23">
+      <c r="A127" t="s">
+        <v>688</v>
+      </c>
       <c r="B127" t="s">
         <v>146</v>
       </c>
@@ -9874,7 +10180,10 @@
         <v>674</v>
       </c>
     </row>
-    <row r="128" spans="2:23">
+    <row r="128" spans="1:23">
+      <c r="A128" t="s">
+        <v>688</v>
+      </c>
       <c r="B128" t="s">
         <v>146</v>
       </c>
@@ -9996,6 +10305,9 @@
       </c>
     </row>
     <row r="131" spans="1:21">
+      <c r="A131" t="s">
+        <v>688</v>
+      </c>
       <c r="B131" t="s">
         <v>197</v>
       </c>
@@ -10043,6 +10355,9 @@
       </c>
     </row>
     <row r="132" spans="1:21">
+      <c r="A132" t="s">
+        <v>688</v>
+      </c>
       <c r="B132" t="s">
         <v>197</v>
       </c>
@@ -10090,6 +10405,9 @@
       </c>
     </row>
     <row r="133" spans="1:21">
+      <c r="A133" t="s">
+        <v>688</v>
+      </c>
       <c r="B133" t="s">
         <v>197</v>
       </c>
@@ -10137,6 +10455,9 @@
       </c>
     </row>
     <row r="134" spans="1:21">
+      <c r="A134" t="s">
+        <v>688</v>
+      </c>
       <c r="B134" t="s">
         <v>197</v>
       </c>
@@ -10184,6 +10505,9 @@
       </c>
     </row>
     <row r="135" spans="1:21">
+      <c r="A135" t="s">
+        <v>688</v>
+      </c>
       <c r="B135" t="s">
         <v>197</v>
       </c>
@@ -10231,6 +10555,9 @@
       </c>
     </row>
     <row r="136" spans="1:21">
+      <c r="A136" t="s">
+        <v>688</v>
+      </c>
       <c r="B136" t="s">
         <v>197</v>
       </c>
@@ -10278,6 +10605,9 @@
       </c>
     </row>
     <row r="137" spans="1:21">
+      <c r="A137" t="s">
+        <v>688</v>
+      </c>
       <c r="B137" t="s">
         <v>197</v>
       </c>
@@ -10325,6 +10655,9 @@
       </c>
     </row>
     <row r="138" spans="1:21">
+      <c r="A138" t="s">
+        <v>688</v>
+      </c>
       <c r="B138" t="s">
         <v>197</v>
       </c>
@@ -10372,6 +10705,9 @@
       </c>
     </row>
     <row r="139" spans="1:21">
+      <c r="A139" t="s">
+        <v>688</v>
+      </c>
       <c r="B139" t="s">
         <v>197</v>
       </c>
@@ -10419,6 +10755,9 @@
       </c>
     </row>
     <row r="140" spans="1:21">
+      <c r="A140" t="s">
+        <v>688</v>
+      </c>
       <c r="B140" t="s">
         <v>197</v>
       </c>
@@ -10466,6 +10805,9 @@
       </c>
     </row>
     <row r="141" spans="1:21">
+      <c r="A141" t="s">
+        <v>688</v>
+      </c>
       <c r="B141" t="s">
         <v>197</v>
       </c>
@@ -10513,6 +10855,9 @@
       </c>
     </row>
     <row r="142" spans="1:21">
+      <c r="A142" t="s">
+        <v>688</v>
+      </c>
       <c r="B142" t="s">
         <v>197</v>
       </c>
@@ -10560,6 +10905,9 @@
       </c>
     </row>
     <row r="143" spans="1:21">
+      <c r="A143" t="s">
+        <v>688</v>
+      </c>
       <c r="B143" t="s">
         <v>197</v>
       </c>
@@ -10607,6 +10955,9 @@
       </c>
     </row>
     <row r="144" spans="1:21">
+      <c r="A144" t="s">
+        <v>688</v>
+      </c>
       <c r="B144" t="s">
         <v>197</v>
       </c>
@@ -10654,6 +11005,9 @@
       </c>
     </row>
     <row r="145" spans="1:16">
+      <c r="A145" t="s">
+        <v>688</v>
+      </c>
       <c r="B145" t="s">
         <v>197</v>
       </c>
@@ -10701,6 +11055,9 @@
       </c>
     </row>
     <row r="146" spans="1:16">
+      <c r="A146" t="s">
+        <v>688</v>
+      </c>
       <c r="B146" t="s">
         <v>197</v>
       </c>
@@ -10748,6 +11105,9 @@
       </c>
     </row>
     <row r="147" spans="1:16">
+      <c r="A147" t="s">
+        <v>688</v>
+      </c>
       <c r="B147" t="s">
         <v>197</v>
       </c>
@@ -10795,6 +11155,9 @@
       </c>
     </row>
     <row r="148" spans="1:16">
+      <c r="A148" t="s">
+        <v>688</v>
+      </c>
       <c r="B148" t="s">
         <v>197</v>
       </c>
@@ -10842,6 +11205,9 @@
       </c>
     </row>
     <row r="149" spans="1:16">
+      <c r="A149" t="s">
+        <v>688</v>
+      </c>
       <c r="B149" t="s">
         <v>197</v>
       </c>
@@ -10939,6 +11305,9 @@
       </c>
     </row>
     <row r="152" spans="1:16">
+      <c r="A152" t="s">
+        <v>688</v>
+      </c>
       <c r="B152" t="s">
         <v>235</v>
       </c>
@@ -10986,6 +11355,9 @@
       </c>
     </row>
     <row r="153" spans="1:16">
+      <c r="A153" t="s">
+        <v>688</v>
+      </c>
       <c r="B153" t="s">
         <v>235</v>
       </c>
@@ -11033,6 +11405,9 @@
       </c>
     </row>
     <row r="154" spans="1:16">
+      <c r="A154" t="s">
+        <v>688</v>
+      </c>
       <c r="B154" t="s">
         <v>235</v>
       </c>
@@ -11080,6 +11455,9 @@
       </c>
     </row>
     <row r="155" spans="1:16">
+      <c r="A155" t="s">
+        <v>688</v>
+      </c>
       <c r="B155" t="s">
         <v>235</v>
       </c>
@@ -11127,6 +11505,9 @@
       </c>
     </row>
     <row r="156" spans="1:16">
+      <c r="A156" t="s">
+        <v>688</v>
+      </c>
       <c r="B156" t="s">
         <v>235</v>
       </c>
@@ -11174,6 +11555,9 @@
       </c>
     </row>
     <row r="157" spans="1:16">
+      <c r="A157" t="s">
+        <v>688</v>
+      </c>
       <c r="B157" t="s">
         <v>235</v>
       </c>
@@ -11221,6 +11605,9 @@
       </c>
     </row>
     <row r="158" spans="1:16">
+      <c r="A158" t="s">
+        <v>688</v>
+      </c>
       <c r="B158" t="s">
         <v>235</v>
       </c>
@@ -11268,6 +11655,9 @@
       </c>
     </row>
     <row r="159" spans="1:16">
+      <c r="A159" t="s">
+        <v>688</v>
+      </c>
       <c r="B159" t="s">
         <v>235</v>
       </c>
@@ -11315,6 +11705,9 @@
       </c>
     </row>
     <row r="160" spans="1:16">
+      <c r="A160" t="s">
+        <v>688</v>
+      </c>
       <c r="B160" t="s">
         <v>235</v>
       </c>
@@ -11361,7 +11754,10 @@
         <v>242</v>
       </c>
     </row>
-    <row r="161" spans="2:16">
+    <row r="161" spans="1:16">
+      <c r="A161" t="s">
+        <v>688</v>
+      </c>
       <c r="B161" t="s">
         <v>235</v>
       </c>
@@ -11408,7 +11804,10 @@
         <v>242</v>
       </c>
     </row>
-    <row r="162" spans="2:16">
+    <row r="162" spans="1:16">
+      <c r="A162" t="s">
+        <v>688</v>
+      </c>
       <c r="B162" t="s">
         <v>235</v>
       </c>
@@ -11455,7 +11854,10 @@
         <v>242</v>
       </c>
     </row>
-    <row r="163" spans="2:16">
+    <row r="163" spans="1:16">
+      <c r="A163" t="s">
+        <v>688</v>
+      </c>
       <c r="B163" t="s">
         <v>235</v>
       </c>
@@ -11502,7 +11904,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="164" spans="2:16">
+    <row r="164" spans="1:16">
+      <c r="A164" t="s">
+        <v>688</v>
+      </c>
       <c r="B164" t="s">
         <v>235</v>
       </c>
@@ -11549,7 +11954,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="165" spans="2:16">
+    <row r="165" spans="1:16">
+      <c r="A165" t="s">
+        <v>688</v>
+      </c>
       <c r="B165" t="s">
         <v>235</v>
       </c>
@@ -11596,7 +12004,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="166" spans="2:16">
+    <row r="166" spans="1:16">
+      <c r="A166" t="s">
+        <v>688</v>
+      </c>
       <c r="B166" t="s">
         <v>235</v>
       </c>
@@ -11643,7 +12054,10 @@
         <v>242</v>
       </c>
     </row>
-    <row r="167" spans="2:16">
+    <row r="167" spans="1:16">
+      <c r="A167" t="s">
+        <v>688</v>
+      </c>
       <c r="B167" t="s">
         <v>235</v>
       </c>
@@ -11690,7 +12104,10 @@
         <v>242</v>
       </c>
     </row>
-    <row r="168" spans="2:16">
+    <row r="168" spans="1:16">
+      <c r="A168" t="s">
+        <v>688</v>
+      </c>
       <c r="B168" t="s">
         <v>235</v>
       </c>
@@ -11737,7 +12154,10 @@
         <v>242</v>
       </c>
     </row>
-    <row r="169" spans="2:16">
+    <row r="169" spans="1:16">
+      <c r="A169" t="s">
+        <v>688</v>
+      </c>
       <c r="B169" t="s">
         <v>235</v>
       </c>
@@ -11784,7 +12204,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="170" spans="2:16">
+    <row r="170" spans="1:16">
+      <c r="A170" t="s">
+        <v>688</v>
+      </c>
       <c r="B170" t="s">
         <v>235</v>
       </c>
@@ -11831,7 +12254,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="171" spans="2:16">
+    <row r="171" spans="1:16">
+      <c r="A171" t="s">
+        <v>688</v>
+      </c>
       <c r="B171" t="s">
         <v>235</v>
       </c>
@@ -11878,7 +12304,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="172" spans="2:16">
+    <row r="172" spans="1:16">
+      <c r="A172" t="s">
+        <v>688</v>
+      </c>
       <c r="B172" t="s">
         <v>235</v>
       </c>
@@ -11925,7 +12354,10 @@
         <v>242</v>
       </c>
     </row>
-    <row r="173" spans="2:16">
+    <row r="173" spans="1:16">
+      <c r="A173" t="s">
+        <v>688</v>
+      </c>
       <c r="B173" t="s">
         <v>235</v>
       </c>
@@ -11972,7 +12404,10 @@
         <v>242</v>
       </c>
     </row>
-    <row r="174" spans="2:16">
+    <row r="174" spans="1:16">
+      <c r="A174" t="s">
+        <v>688</v>
+      </c>
       <c r="B174" t="s">
         <v>235</v>
       </c>
@@ -12019,7 +12454,10 @@
         <v>242</v>
       </c>
     </row>
-    <row r="175" spans="2:16">
+    <row r="175" spans="1:16">
+      <c r="A175" t="s">
+        <v>688</v>
+      </c>
       <c r="B175" t="s">
         <v>235</v>
       </c>
@@ -12066,7 +12504,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="176" spans="2:16">
+    <row r="176" spans="1:16">
+      <c r="A176" t="s">
+        <v>688</v>
+      </c>
       <c r="B176" t="s">
         <v>235</v>
       </c>
@@ -12114,6 +12555,9 @@
       </c>
     </row>
     <row r="177" spans="1:16">
+      <c r="A177" t="s">
+        <v>688</v>
+      </c>
       <c r="B177" t="s">
         <v>235</v>
       </c>
@@ -12161,6 +12605,9 @@
       </c>
     </row>
     <row r="178" spans="1:16">
+      <c r="A178" t="s">
+        <v>688</v>
+      </c>
       <c r="B178" t="s">
         <v>235</v>
       </c>
@@ -12208,6 +12655,9 @@
       </c>
     </row>
     <row r="179" spans="1:16">
+      <c r="A179" t="s">
+        <v>688</v>
+      </c>
       <c r="B179" t="s">
         <v>235</v>
       </c>
@@ -12255,6 +12705,9 @@
       </c>
     </row>
     <row r="180" spans="1:16">
+      <c r="A180" t="s">
+        <v>688</v>
+      </c>
       <c r="B180" t="s">
         <v>235</v>
       </c>
@@ -12352,6 +12805,9 @@
       </c>
     </row>
     <row r="183" spans="1:16">
+      <c r="A183" t="s">
+        <v>689</v>
+      </c>
       <c r="B183" t="s">
         <v>243</v>
       </c>
@@ -12399,6 +12855,9 @@
       </c>
     </row>
     <row r="184" spans="1:16">
+      <c r="A184" t="s">
+        <v>689</v>
+      </c>
       <c r="B184" t="s">
         <v>243</v>
       </c>
@@ -12446,6 +12905,9 @@
       </c>
     </row>
     <row r="185" spans="1:16">
+      <c r="A185" t="s">
+        <v>689</v>
+      </c>
       <c r="B185" t="s">
         <v>243</v>
       </c>
@@ -12493,6 +12955,9 @@
       </c>
     </row>
     <row r="186" spans="1:16">
+      <c r="A186" t="s">
+        <v>689</v>
+      </c>
       <c r="B186" t="s">
         <v>243</v>
       </c>
@@ -12590,6 +13055,9 @@
       </c>
     </row>
     <row r="189" spans="1:16">
+      <c r="A189" t="s">
+        <v>688</v>
+      </c>
       <c r="B189" t="s">
         <v>248</v>
       </c>
@@ -12637,6 +13105,9 @@
       </c>
     </row>
     <row r="190" spans="1:16">
+      <c r="A190" t="s">
+        <v>688</v>
+      </c>
       <c r="B190" t="s">
         <v>248</v>
       </c>
@@ -12684,6 +13155,9 @@
       </c>
     </row>
     <row r="191" spans="1:16">
+      <c r="A191" t="s">
+        <v>688</v>
+      </c>
       <c r="B191" t="s">
         <v>248</v>
       </c>
@@ -12781,6 +13255,9 @@
       </c>
     </row>
     <row r="194" spans="1:16">
+      <c r="A194" t="s">
+        <v>688</v>
+      </c>
       <c r="B194" t="s">
         <v>258</v>
       </c>
@@ -12828,6 +13305,9 @@
       </c>
     </row>
     <row r="195" spans="1:16">
+      <c r="A195" t="s">
+        <v>688</v>
+      </c>
       <c r="B195" t="s">
         <v>258</v>
       </c>
@@ -12875,6 +13355,9 @@
       </c>
     </row>
     <row r="196" spans="1:16">
+      <c r="A196" t="s">
+        <v>688</v>
+      </c>
       <c r="B196" t="s">
         <v>258</v>
       </c>
@@ -12922,6 +13405,9 @@
       </c>
     </row>
     <row r="197" spans="1:16">
+      <c r="A197" t="s">
+        <v>688</v>
+      </c>
       <c r="B197" t="s">
         <v>258</v>
       </c>
@@ -12969,6 +13455,9 @@
       </c>
     </row>
     <row r="198" spans="1:16">
+      <c r="A198" t="s">
+        <v>688</v>
+      </c>
       <c r="B198" t="s">
         <v>258</v>
       </c>
@@ -13016,6 +13505,9 @@
       </c>
     </row>
     <row r="199" spans="1:16">
+      <c r="A199" t="s">
+        <v>688</v>
+      </c>
       <c r="B199" t="s">
         <v>258</v>
       </c>
@@ -13063,6 +13555,9 @@
       </c>
     </row>
     <row r="200" spans="1:16">
+      <c r="A200" t="s">
+        <v>688</v>
+      </c>
       <c r="B200" t="s">
         <v>258</v>
       </c>
@@ -13110,6 +13605,9 @@
       </c>
     </row>
     <row r="201" spans="1:16">
+      <c r="A201" t="s">
+        <v>688</v>
+      </c>
       <c r="B201" t="s">
         <v>258</v>
       </c>
@@ -13157,6 +13655,9 @@
       </c>
     </row>
     <row r="202" spans="1:16">
+      <c r="A202" t="s">
+        <v>688</v>
+      </c>
       <c r="B202" t="s">
         <v>258</v>
       </c>
@@ -13254,6 +13755,9 @@
       </c>
     </row>
     <row r="205" spans="1:16">
+      <c r="A205" t="s">
+        <v>687</v>
+      </c>
       <c r="B205" t="s">
         <v>281</v>
       </c>
@@ -13301,6 +13805,9 @@
       </c>
     </row>
     <row r="206" spans="1:16">
+      <c r="A206" t="s">
+        <v>687</v>
+      </c>
       <c r="B206" t="s">
         <v>281</v>
       </c>
@@ -13348,6 +13855,9 @@
       </c>
     </row>
     <row r="207" spans="1:16">
+      <c r="A207" t="s">
+        <v>687</v>
+      </c>
       <c r="B207" t="s">
         <v>281</v>
       </c>
@@ -13395,6 +13905,9 @@
       </c>
     </row>
     <row r="208" spans="1:16">
+      <c r="A208" t="s">
+        <v>687</v>
+      </c>
       <c r="B208" t="s">
         <v>281</v>
       </c>
@@ -13442,6 +13955,9 @@
       </c>
     </row>
     <row r="209" spans="1:23">
+      <c r="A209" t="s">
+        <v>687</v>
+      </c>
       <c r="B209" t="s">
         <v>281</v>
       </c>
@@ -13539,6 +14055,9 @@
       </c>
     </row>
     <row r="212" spans="1:23">
+      <c r="A212" t="s">
+        <v>687</v>
+      </c>
       <c r="B212" t="s">
         <v>296</v>
       </c>
@@ -13586,6 +14105,9 @@
       </c>
     </row>
     <row r="213" spans="1:23">
+      <c r="A213" t="s">
+        <v>687</v>
+      </c>
       <c r="B213" t="s">
         <v>296</v>
       </c>
@@ -13633,6 +14155,9 @@
       </c>
     </row>
     <row r="214" spans="1:23">
+      <c r="A214" t="s">
+        <v>687</v>
+      </c>
       <c r="B214" t="s">
         <v>296</v>
       </c>
@@ -13680,6 +14205,9 @@
       </c>
     </row>
     <row r="215" spans="1:23">
+      <c r="A215" t="s">
+        <v>687</v>
+      </c>
       <c r="B215" t="s">
         <v>296</v>
       </c>
@@ -13727,6 +14255,9 @@
       </c>
     </row>
     <row r="216" spans="1:23">
+      <c r="A216" t="s">
+        <v>687</v>
+      </c>
       <c r="B216" t="s">
         <v>296</v>
       </c>
@@ -13774,6 +14305,9 @@
       </c>
     </row>
     <row r="217" spans="1:23">
+      <c r="A217" t="s">
+        <v>687</v>
+      </c>
       <c r="B217" t="s">
         <v>296</v>
       </c>
@@ -13821,6 +14355,9 @@
       </c>
     </row>
     <row r="218" spans="1:23">
+      <c r="A218" t="s">
+        <v>687</v>
+      </c>
       <c r="B218" t="s">
         <v>296</v>
       </c>
@@ -14060,6 +14597,9 @@
       </c>
     </row>
     <row r="224" spans="1:23">
+      <c r="A224" t="s">
+        <v>688</v>
+      </c>
       <c r="B224" t="s">
         <v>306</v>
       </c>
@@ -14110,6 +14650,9 @@
       </c>
     </row>
     <row r="225" spans="1:23">
+      <c r="A225" t="s">
+        <v>688</v>
+      </c>
       <c r="B225" t="s">
         <v>306</v>
       </c>
@@ -14160,6 +14703,9 @@
       </c>
     </row>
     <row r="226" spans="1:23">
+      <c r="A226" t="s">
+        <v>688</v>
+      </c>
       <c r="B226" t="s">
         <v>306</v>
       </c>
@@ -14210,6 +14756,9 @@
       </c>
     </row>
     <row r="227" spans="1:23">
+      <c r="A227" t="s">
+        <v>688</v>
+      </c>
       <c r="B227" t="s">
         <v>306</v>
       </c>
@@ -14331,6 +14880,9 @@
       </c>
     </row>
     <row r="229" spans="1:23">
+      <c r="A229" t="s">
+        <v>687</v>
+      </c>
       <c r="B229" t="s">
         <v>306</v>
       </c>
@@ -14399,6 +14951,9 @@
       </c>
     </row>
     <row r="230" spans="1:23">
+      <c r="A230" t="s">
+        <v>687</v>
+      </c>
       <c r="B230" t="s">
         <v>306</v>
       </c>
@@ -14467,6 +15022,9 @@
       </c>
     </row>
     <row r="231" spans="1:23">
+      <c r="A231" t="s">
+        <v>687</v>
+      </c>
       <c r="B231" t="s">
         <v>306</v>
       </c>
@@ -14535,6 +15093,9 @@
       </c>
     </row>
     <row r="232" spans="1:23">
+      <c r="A232" t="s">
+        <v>687</v>
+      </c>
       <c r="B232" t="s">
         <v>306</v>
       </c>
@@ -14603,6 +15164,9 @@
       </c>
     </row>
     <row r="233" spans="1:23">
+      <c r="A233" t="s">
+        <v>687</v>
+      </c>
       <c r="B233" t="s">
         <v>306</v>
       </c>
@@ -14671,6 +15235,9 @@
       </c>
     </row>
     <row r="234" spans="1:23">
+      <c r="A234" t="s">
+        <v>687</v>
+      </c>
       <c r="B234" t="s">
         <v>306</v>
       </c>
@@ -14739,6 +15306,9 @@
       </c>
     </row>
     <row r="235" spans="1:23">
+      <c r="A235" t="s">
+        <v>687</v>
+      </c>
       <c r="B235" t="s">
         <v>306</v>
       </c>
@@ -14807,6 +15377,9 @@
       </c>
     </row>
     <row r="236" spans="1:23">
+      <c r="A236" t="s">
+        <v>687</v>
+      </c>
       <c r="B236" t="s">
         <v>306</v>
       </c>
@@ -14875,6 +15448,9 @@
       </c>
     </row>
     <row r="237" spans="1:23">
+      <c r="A237" t="s">
+        <v>687</v>
+      </c>
       <c r="B237" t="s">
         <v>306</v>
       </c>
@@ -14943,6 +15519,9 @@
       </c>
     </row>
     <row r="238" spans="1:23">
+      <c r="A238" t="s">
+        <v>687</v>
+      </c>
       <c r="B238" t="s">
         <v>306</v>
       </c>
@@ -15011,6 +15590,9 @@
       </c>
     </row>
     <row r="239" spans="1:23">
+      <c r="A239" t="s">
+        <v>687</v>
+      </c>
       <c r="B239" t="s">
         <v>306</v>
       </c>
@@ -15079,6 +15661,9 @@
       </c>
     </row>
     <row r="240" spans="1:23">
+      <c r="A240" t="s">
+        <v>687</v>
+      </c>
       <c r="B240" t="s">
         <v>306</v>
       </c>
@@ -15147,6 +15732,9 @@
       </c>
     </row>
     <row r="241" spans="1:23">
+      <c r="A241" t="s">
+        <v>687</v>
+      </c>
       <c r="B241" t="s">
         <v>306</v>
       </c>
@@ -15215,6 +15803,9 @@
       </c>
     </row>
     <row r="242" spans="1:23">
+      <c r="A242" t="s">
+        <v>687</v>
+      </c>
       <c r="B242" t="s">
         <v>306</v>
       </c>
@@ -15283,6 +15874,9 @@
       </c>
     </row>
     <row r="243" spans="1:23">
+      <c r="A243" t="s">
+        <v>687</v>
+      </c>
       <c r="B243" t="s">
         <v>306</v>
       </c>
@@ -15407,6 +16001,9 @@
       </c>
     </row>
     <row r="247" spans="1:23">
+      <c r="A247" t="s">
+        <v>688</v>
+      </c>
       <c r="B247" t="s">
         <v>326</v>
       </c>
@@ -15504,6 +16101,9 @@
       </c>
     </row>
     <row r="250" spans="1:23">
+      <c r="A250" t="s">
+        <v>687</v>
+      </c>
       <c r="B250" t="s">
         <v>330</v>
       </c>
@@ -15551,6 +16151,9 @@
       </c>
     </row>
     <row r="251" spans="1:23">
+      <c r="A251" t="s">
+        <v>687</v>
+      </c>
       <c r="B251" t="s">
         <v>330</v>
       </c>
@@ -15598,6 +16201,9 @@
       </c>
     </row>
     <row r="252" spans="1:23">
+      <c r="A252" t="s">
+        <v>687</v>
+      </c>
       <c r="B252" t="s">
         <v>330</v>
       </c>
@@ -15645,6 +16251,9 @@
       </c>
     </row>
     <row r="253" spans="1:23">
+      <c r="A253" t="s">
+        <v>687</v>
+      </c>
       <c r="B253" t="s">
         <v>330</v>
       </c>
@@ -15692,6 +16301,9 @@
       </c>
     </row>
     <row r="254" spans="1:23">
+      <c r="A254" t="s">
+        <v>687</v>
+      </c>
       <c r="B254" t="s">
         <v>330</v>
       </c>
@@ -15739,6 +16351,9 @@
       </c>
     </row>
     <row r="255" spans="1:23">
+      <c r="A255" t="s">
+        <v>687</v>
+      </c>
       <c r="B255" t="s">
         <v>330</v>
       </c>
@@ -15786,6 +16401,9 @@
       </c>
     </row>
     <row r="256" spans="1:23">
+      <c r="A256" t="s">
+        <v>687</v>
+      </c>
       <c r="B256" t="s">
         <v>330</v>
       </c>
@@ -15907,6 +16525,9 @@
       </c>
     </row>
     <row r="259" spans="1:23">
+      <c r="A259" t="s">
+        <v>689</v>
+      </c>
       <c r="B259" t="s">
         <v>339</v>
       </c>
@@ -15975,6 +16596,9 @@
       </c>
     </row>
     <row r="260" spans="1:23">
+      <c r="A260" t="s">
+        <v>689</v>
+      </c>
       <c r="B260" t="s">
         <v>339</v>
       </c>
@@ -16049,6 +16673,9 @@
       <c r="U261" s="1"/>
     </row>
     <row r="262" spans="1:23">
+      <c r="A262" t="s">
+        <v>689</v>
+      </c>
       <c r="B262" t="s">
         <v>339</v>
       </c>
@@ -16117,6 +16744,9 @@
       </c>
     </row>
     <row r="263" spans="1:23">
+      <c r="A263" t="s">
+        <v>689</v>
+      </c>
       <c r="B263" t="s">
         <v>339</v>
       </c>
@@ -16185,6 +16815,9 @@
       </c>
     </row>
     <row r="264" spans="1:23">
+      <c r="A264" t="s">
+        <v>689</v>
+      </c>
       <c r="B264" t="s">
         <v>339</v>
       </c>
@@ -16253,6 +16886,9 @@
       </c>
     </row>
     <row r="265" spans="1:23">
+      <c r="A265" t="s">
+        <v>689</v>
+      </c>
       <c r="B265" t="s">
         <v>339</v>
       </c>
@@ -16321,6 +16957,9 @@
       </c>
     </row>
     <row r="266" spans="1:23">
+      <c r="A266" t="s">
+        <v>689</v>
+      </c>
       <c r="B266" t="s">
         <v>339</v>
       </c>
@@ -16389,6 +17028,9 @@
       </c>
     </row>
     <row r="267" spans="1:23">
+      <c r="A267" t="s">
+        <v>689</v>
+      </c>
       <c r="B267" t="s">
         <v>339</v>
       </c>
@@ -16457,6 +17099,9 @@
       </c>
     </row>
     <row r="268" spans="1:23">
+      <c r="A268" t="s">
+        <v>689</v>
+      </c>
       <c r="B268" t="s">
         <v>339</v>
       </c>
@@ -16525,6 +17170,9 @@
       </c>
     </row>
     <row r="269" spans="1:23">
+      <c r="A269" t="s">
+        <v>689</v>
+      </c>
       <c r="B269" t="s">
         <v>339</v>
       </c>
@@ -16593,6 +17241,9 @@
       </c>
     </row>
     <row r="270" spans="1:23">
+      <c r="A270" t="s">
+        <v>689</v>
+      </c>
       <c r="B270" t="s">
         <v>339</v>
       </c>
@@ -16661,6 +17312,9 @@
       </c>
     </row>
     <row r="271" spans="1:23">
+      <c r="A271" t="s">
+        <v>689</v>
+      </c>
       <c r="B271" t="s">
         <v>339</v>
       </c>
@@ -16803,6 +17457,9 @@
       </c>
     </row>
     <row r="274" spans="1:23">
+      <c r="A274" t="s">
+        <v>689</v>
+      </c>
       <c r="B274" t="s">
         <v>357</v>
       </c>
@@ -16871,6 +17528,9 @@
       </c>
     </row>
     <row r="275" spans="1:23">
+      <c r="A275" t="s">
+        <v>689</v>
+      </c>
       <c r="B275" t="s">
         <v>357</v>
       </c>
@@ -16939,6 +17599,9 @@
       </c>
     </row>
     <row r="276" spans="1:23">
+      <c r="A276" t="s">
+        <v>689</v>
+      </c>
       <c r="B276" t="s">
         <v>357</v>
       </c>
@@ -17007,6 +17670,9 @@
       </c>
     </row>
     <row r="277" spans="1:23">
+      <c r="A277" t="s">
+        <v>689</v>
+      </c>
       <c r="B277" t="s">
         <v>357</v>
       </c>
@@ -17075,6 +17741,9 @@
       </c>
     </row>
     <row r="278" spans="1:23">
+      <c r="A278" t="s">
+        <v>689</v>
+      </c>
       <c r="B278" t="s">
         <v>357</v>
       </c>
@@ -17196,6 +17865,9 @@
       </c>
     </row>
     <row r="281" spans="1:23">
+      <c r="A281" t="s">
+        <v>689</v>
+      </c>
       <c r="B281" t="s">
         <v>358</v>
       </c>
@@ -17243,6 +17915,9 @@
       </c>
     </row>
     <row r="282" spans="1:23">
+      <c r="A282" t="s">
+        <v>689</v>
+      </c>
       <c r="B282" t="s">
         <v>358</v>
       </c>
@@ -17290,6 +17965,9 @@
       </c>
     </row>
     <row r="283" spans="1:23">
+      <c r="A283" t="s">
+        <v>689</v>
+      </c>
       <c r="B283" t="s">
         <v>358</v>
       </c>
@@ -17337,6 +18015,9 @@
       </c>
     </row>
     <row r="284" spans="1:23">
+      <c r="A284" t="s">
+        <v>689</v>
+      </c>
       <c r="B284" t="s">
         <v>358</v>
       </c>
@@ -17384,6 +18065,9 @@
       </c>
     </row>
     <row r="285" spans="1:23">
+      <c r="A285" t="s">
+        <v>689</v>
+      </c>
       <c r="B285" t="s">
         <v>358</v>
       </c>
@@ -17499,6 +18183,9 @@
       </c>
     </row>
     <row r="289" spans="1:23">
+      <c r="A289" t="s">
+        <v>689</v>
+      </c>
       <c r="B289" t="s">
         <v>375</v>
       </c>
@@ -17611,6 +18298,9 @@
       </c>
     </row>
     <row r="292" spans="1:23">
+      <c r="A292" t="s">
+        <v>689</v>
+      </c>
       <c r="B292" t="s">
         <v>378</v>
       </c>
@@ -17663,6 +18353,9 @@
       </c>
     </row>
     <row r="294" spans="1:23">
+      <c r="A294" t="s">
+        <v>689</v>
+      </c>
       <c r="B294" t="s">
         <v>378</v>
       </c>
@@ -17710,6 +18403,9 @@
       </c>
     </row>
     <row r="295" spans="1:23">
+      <c r="A295" t="s">
+        <v>689</v>
+      </c>
       <c r="B295" t="s">
         <v>378</v>
       </c>
@@ -17757,6 +18453,9 @@
       </c>
     </row>
     <row r="296" spans="1:23">
+      <c r="A296" t="s">
+        <v>689</v>
+      </c>
       <c r="B296" t="s">
         <v>378</v>
       </c>
@@ -17804,6 +18503,9 @@
       </c>
     </row>
     <row r="297" spans="1:23">
+      <c r="A297" t="s">
+        <v>689</v>
+      </c>
       <c r="B297" t="s">
         <v>378</v>
       </c>
@@ -17851,6 +18553,9 @@
       </c>
     </row>
     <row r="298" spans="1:23">
+      <c r="A298" t="s">
+        <v>689</v>
+      </c>
       <c r="B298" t="s">
         <v>378</v>
       </c>
@@ -17898,6 +18603,9 @@
       </c>
     </row>
     <row r="299" spans="1:23">
+      <c r="A299" t="s">
+        <v>689</v>
+      </c>
       <c r="B299" t="s">
         <v>378</v>
       </c>
@@ -17945,6 +18653,9 @@
       </c>
     </row>
     <row r="300" spans="1:23">
+      <c r="A300" t="s">
+        <v>689</v>
+      </c>
       <c r="B300" t="s">
         <v>378</v>
       </c>
@@ -17992,6 +18703,9 @@
       </c>
     </row>
     <row r="301" spans="1:23">
+      <c r="A301" t="s">
+        <v>689</v>
+      </c>
       <c r="B301" t="s">
         <v>378</v>
       </c>
@@ -18039,6 +18753,9 @@
       </c>
     </row>
     <row r="302" spans="1:23">
+      <c r="A302" t="s">
+        <v>689</v>
+      </c>
       <c r="B302" t="s">
         <v>378</v>
       </c>
@@ -18086,6 +18803,9 @@
       </c>
     </row>
     <row r="303" spans="1:23">
+      <c r="A303" t="s">
+        <v>689</v>
+      </c>
       <c r="B303" t="s">
         <v>378</v>
       </c>
@@ -18133,6 +18853,9 @@
       </c>
     </row>
     <row r="304" spans="1:23">
+      <c r="A304" t="s">
+        <v>689</v>
+      </c>
       <c r="B304" t="s">
         <v>378</v>
       </c>
@@ -18230,6 +18953,9 @@
       </c>
     </row>
     <row r="307" spans="1:23">
+      <c r="A307" t="s">
+        <v>689</v>
+      </c>
       <c r="B307" t="s">
         <v>388</v>
       </c>
@@ -18277,6 +19003,9 @@
       </c>
     </row>
     <row r="308" spans="1:23">
+      <c r="A308" t="s">
+        <v>689</v>
+      </c>
       <c r="B308" t="s">
         <v>388</v>
       </c>
@@ -18324,6 +19053,9 @@
       </c>
     </row>
     <row r="309" spans="1:23">
+      <c r="A309" t="s">
+        <v>689</v>
+      </c>
       <c r="B309" t="s">
         <v>388</v>
       </c>
@@ -18371,6 +19103,9 @@
       </c>
     </row>
     <row r="310" spans="1:23">
+      <c r="A310" t="s">
+        <v>689</v>
+      </c>
       <c r="B310" t="s">
         <v>388</v>
       </c>
@@ -18418,6 +19153,9 @@
       </c>
     </row>
     <row r="311" spans="1:23">
+      <c r="A311" t="s">
+        <v>689</v>
+      </c>
       <c r="B311" t="s">
         <v>388</v>
       </c>
@@ -18465,6 +19203,9 @@
       </c>
     </row>
     <row r="312" spans="1:23">
+      <c r="A312" t="s">
+        <v>689</v>
+      </c>
       <c r="B312" t="s">
         <v>388</v>
       </c>
@@ -18512,6 +19253,9 @@
       </c>
     </row>
     <row r="313" spans="1:23">
+      <c r="A313" t="s">
+        <v>689</v>
+      </c>
       <c r="B313" t="s">
         <v>388</v>
       </c>
@@ -18559,6 +19303,9 @@
       </c>
     </row>
     <row r="314" spans="1:23">
+      <c r="A314" t="s">
+        <v>689</v>
+      </c>
       <c r="B314" t="s">
         <v>388</v>
       </c>
@@ -18606,6 +19353,9 @@
       </c>
     </row>
     <row r="315" spans="1:23">
+      <c r="A315" t="s">
+        <v>689</v>
+      </c>
       <c r="B315" t="s">
         <v>388</v>
       </c>
@@ -18730,6 +19480,9 @@
       </c>
     </row>
     <row r="319" spans="1:23">
+      <c r="A319" t="s">
+        <v>689</v>
+      </c>
       <c r="B319" t="s">
         <v>391</v>
       </c>
@@ -18798,6 +19551,9 @@
       </c>
     </row>
     <row r="320" spans="1:23">
+      <c r="A320" t="s">
+        <v>689</v>
+      </c>
       <c r="B320" t="s">
         <v>391</v>
       </c>
@@ -18865,7 +19621,10 @@
         <v>673</v>
       </c>
     </row>
-    <row r="321" spans="2:23">
+    <row r="321" spans="1:23">
+      <c r="A321" t="s">
+        <v>689</v>
+      </c>
       <c r="B321" t="s">
         <v>391</v>
       </c>
@@ -18933,7 +19692,10 @@
         <v>673</v>
       </c>
     </row>
-    <row r="322" spans="2:23">
+    <row r="322" spans="1:23">
+      <c r="A322" t="s">
+        <v>689</v>
+      </c>
       <c r="B322" t="s">
         <v>391</v>
       </c>
@@ -19001,7 +19763,10 @@
         <v>673</v>
       </c>
     </row>
-    <row r="323" spans="2:23">
+    <row r="323" spans="1:23">
+      <c r="A323" t="s">
+        <v>689</v>
+      </c>
       <c r="B323" t="s">
         <v>391</v>
       </c>
@@ -19069,7 +19834,10 @@
         <v>673</v>
       </c>
     </row>
-    <row r="324" spans="2:23">
+    <row r="324" spans="1:23">
+      <c r="A324" t="s">
+        <v>689</v>
+      </c>
       <c r="B324" t="s">
         <v>391</v>
       </c>
@@ -19137,7 +19905,10 @@
         <v>673</v>
       </c>
     </row>
-    <row r="325" spans="2:23">
+    <row r="325" spans="1:23">
+      <c r="A325" t="s">
+        <v>689</v>
+      </c>
       <c r="B325" t="s">
         <v>391</v>
       </c>
@@ -19202,7 +19973,10 @@
         <v>673</v>
       </c>
     </row>
-    <row r="326" spans="2:23">
+    <row r="326" spans="1:23">
+      <c r="A326" t="s">
+        <v>689</v>
+      </c>
       <c r="B326" t="s">
         <v>391</v>
       </c>
@@ -19270,7 +20044,10 @@
         <v>673</v>
       </c>
     </row>
-    <row r="327" spans="2:23">
+    <row r="327" spans="1:23">
+      <c r="A327" t="s">
+        <v>689</v>
+      </c>
       <c r="B327" t="s">
         <v>391</v>
       </c>
@@ -19338,7 +20115,10 @@
         <v>673</v>
       </c>
     </row>
-    <row r="328" spans="2:23">
+    <row r="328" spans="1:23">
+      <c r="A328" t="s">
+        <v>689</v>
+      </c>
       <c r="B328" t="s">
         <v>391</v>
       </c>
@@ -19406,7 +20186,10 @@
         <v>673</v>
       </c>
     </row>
-    <row r="329" spans="2:23">
+    <row r="329" spans="1:23">
+      <c r="A329" t="s">
+        <v>689</v>
+      </c>
       <c r="B329" t="s">
         <v>391</v>
       </c>
@@ -19474,7 +20257,10 @@
         <v>673</v>
       </c>
     </row>
-    <row r="330" spans="2:23">
+    <row r="330" spans="1:23">
+      <c r="A330" t="s">
+        <v>689</v>
+      </c>
       <c r="B330" t="s">
         <v>391</v>
       </c>
@@ -19542,7 +20328,10 @@
         <v>673</v>
       </c>
     </row>
-    <row r="331" spans="2:23">
+    <row r="331" spans="1:23">
+      <c r="A331" t="s">
+        <v>689</v>
+      </c>
       <c r="B331" t="s">
         <v>391</v>
       </c>
@@ -19610,7 +20399,10 @@
         <v>673</v>
       </c>
     </row>
-    <row r="332" spans="2:23">
+    <row r="332" spans="1:23">
+      <c r="A332" t="s">
+        <v>689</v>
+      </c>
       <c r="B332" t="s">
         <v>391</v>
       </c>
@@ -19678,7 +20470,10 @@
         <v>673</v>
       </c>
     </row>
-    <row r="333" spans="2:23">
+    <row r="333" spans="1:23">
+      <c r="A333" t="s">
+        <v>689</v>
+      </c>
       <c r="B333" t="s">
         <v>391</v>
       </c>
@@ -19746,7 +20541,10 @@
         <v>673</v>
       </c>
     </row>
-    <row r="334" spans="2:23">
+    <row r="334" spans="1:23">
+      <c r="A334" t="s">
+        <v>689</v>
+      </c>
       <c r="B334" t="s">
         <v>391</v>
       </c>
@@ -19814,7 +20612,10 @@
         <v>673</v>
       </c>
     </row>
-    <row r="335" spans="2:23">
+    <row r="335" spans="1:23">
+      <c r="A335" t="s">
+        <v>689</v>
+      </c>
       <c r="B335" t="s">
         <v>391</v>
       </c>
@@ -19882,7 +20683,10 @@
         <v>673</v>
       </c>
     </row>
-    <row r="336" spans="2:23">
+    <row r="336" spans="1:23">
+      <c r="A336" t="s">
+        <v>689</v>
+      </c>
       <c r="B336" t="s">
         <v>391</v>
       </c>
@@ -19950,7 +20754,10 @@
         <v>673</v>
       </c>
     </row>
-    <row r="337" spans="2:23">
+    <row r="337" spans="1:23">
+      <c r="A337" t="s">
+        <v>689</v>
+      </c>
       <c r="B337" t="s">
         <v>391</v>
       </c>
@@ -20018,7 +20825,10 @@
         <v>673</v>
       </c>
     </row>
-    <row r="338" spans="2:23">
+    <row r="338" spans="1:23">
+      <c r="A338" t="s">
+        <v>689</v>
+      </c>
       <c r="B338" t="s">
         <v>391</v>
       </c>
@@ -20086,7 +20896,10 @@
         <v>673</v>
       </c>
     </row>
-    <row r="339" spans="2:23">
+    <row r="339" spans="1:23">
+      <c r="A339" t="s">
+        <v>689</v>
+      </c>
       <c r="B339" t="s">
         <v>391</v>
       </c>
@@ -20154,7 +20967,10 @@
         <v>673</v>
       </c>
     </row>
-    <row r="340" spans="2:23">
+    <row r="340" spans="1:23">
+      <c r="A340" t="s">
+        <v>689</v>
+      </c>
       <c r="B340" t="s">
         <v>391</v>
       </c>
@@ -20222,7 +21038,10 @@
         <v>673</v>
       </c>
     </row>
-    <row r="341" spans="2:23">
+    <row r="341" spans="1:23">
+      <c r="A341" t="s">
+        <v>689</v>
+      </c>
       <c r="B341" t="s">
         <v>391</v>
       </c>
@@ -20290,7 +21109,10 @@
         <v>673</v>
       </c>
     </row>
-    <row r="342" spans="2:23">
+    <row r="342" spans="1:23">
+      <c r="A342" t="s">
+        <v>689</v>
+      </c>
       <c r="B342" t="s">
         <v>391</v>
       </c>
@@ -20358,7 +21180,10 @@
         <v>673</v>
       </c>
     </row>
-    <row r="343" spans="2:23">
+    <row r="343" spans="1:23">
+      <c r="A343" t="s">
+        <v>689</v>
+      </c>
       <c r="B343" t="s">
         <v>391</v>
       </c>
@@ -20426,7 +21251,10 @@
         <v>673</v>
       </c>
     </row>
-    <row r="344" spans="2:23">
+    <row r="344" spans="1:23">
+      <c r="A344" t="s">
+        <v>689</v>
+      </c>
       <c r="B344" t="s">
         <v>391</v>
       </c>
@@ -20494,7 +21322,10 @@
         <v>673</v>
       </c>
     </row>
-    <row r="345" spans="2:23">
+    <row r="345" spans="1:23">
+      <c r="A345" t="s">
+        <v>689</v>
+      </c>
       <c r="B345" t="s">
         <v>391</v>
       </c>
@@ -20562,7 +21393,10 @@
         <v>673</v>
       </c>
     </row>
-    <row r="346" spans="2:23">
+    <row r="346" spans="1:23">
+      <c r="A346" t="s">
+        <v>689</v>
+      </c>
       <c r="B346" t="s">
         <v>391</v>
       </c>
@@ -20630,7 +21464,10 @@
         <v>673</v>
       </c>
     </row>
-    <row r="347" spans="2:23">
+    <row r="347" spans="1:23">
+      <c r="A347" t="s">
+        <v>689</v>
+      </c>
       <c r="B347" t="s">
         <v>391</v>
       </c>
@@ -20698,7 +21535,10 @@
         <v>673</v>
       </c>
     </row>
-    <row r="348" spans="2:23">
+    <row r="348" spans="1:23">
+      <c r="A348" t="s">
+        <v>689</v>
+      </c>
       <c r="B348" t="s">
         <v>391</v>
       </c>
@@ -20766,7 +21606,10 @@
         <v>673</v>
       </c>
     </row>
-    <row r="349" spans="2:23">
+    <row r="349" spans="1:23">
+      <c r="A349" t="s">
+        <v>689</v>
+      </c>
       <c r="B349" t="s">
         <v>391</v>
       </c>
@@ -20834,7 +21677,10 @@
         <v>673</v>
       </c>
     </row>
-    <row r="350" spans="2:23">
+    <row r="350" spans="1:23">
+      <c r="A350" t="s">
+        <v>689</v>
+      </c>
       <c r="B350" t="s">
         <v>391</v>
       </c>
@@ -20902,7 +21748,10 @@
         <v>673</v>
       </c>
     </row>
-    <row r="351" spans="2:23">
+    <row r="351" spans="1:23">
+      <c r="A351" t="s">
+        <v>689</v>
+      </c>
       <c r="B351" t="s">
         <v>391</v>
       </c>
@@ -20970,7 +21819,10 @@
         <v>673</v>
       </c>
     </row>
-    <row r="352" spans="2:23">
+    <row r="352" spans="1:23">
+      <c r="A352" t="s">
+        <v>689</v>
+      </c>
       <c r="B352" t="s">
         <v>391</v>
       </c>
@@ -21039,6 +21891,9 @@
       </c>
     </row>
     <row r="353" spans="1:23">
+      <c r="A353" t="s">
+        <v>689</v>
+      </c>
       <c r="B353" t="s">
         <v>391</v>
       </c>
@@ -21107,6 +21962,9 @@
       </c>
     </row>
     <row r="354" spans="1:23">
+      <c r="A354" t="s">
+        <v>689</v>
+      </c>
       <c r="B354" t="s">
         <v>391</v>
       </c>
@@ -21175,6 +22033,9 @@
       </c>
     </row>
     <row r="355" spans="1:23">
+      <c r="A355" t="s">
+        <v>689</v>
+      </c>
       <c r="B355" t="s">
         <v>391</v>
       </c>
@@ -21243,6 +22104,9 @@
       </c>
     </row>
     <row r="356" spans="1:23">
+      <c r="A356" t="s">
+        <v>689</v>
+      </c>
       <c r="B356" t="s">
         <v>391</v>
       </c>
@@ -21311,6 +22175,9 @@
       </c>
     </row>
     <row r="357" spans="1:23">
+      <c r="A357" t="s">
+        <v>689</v>
+      </c>
       <c r="B357" t="s">
         <v>391</v>
       </c>
@@ -21379,6 +22246,9 @@
       </c>
     </row>
     <row r="358" spans="1:23">
+      <c r="A358" t="s">
+        <v>689</v>
+      </c>
       <c r="B358" t="s">
         <v>391</v>
       </c>
@@ -21447,6 +22317,9 @@
       </c>
     </row>
     <row r="359" spans="1:23">
+      <c r="A359" t="s">
+        <v>689</v>
+      </c>
       <c r="B359" t="s">
         <v>391</v>
       </c>
@@ -21515,6 +22388,9 @@
       </c>
     </row>
     <row r="360" spans="1:23">
+      <c r="A360" t="s">
+        <v>689</v>
+      </c>
       <c r="B360" t="s">
         <v>391</v>
       </c>
@@ -21583,6 +22459,9 @@
       </c>
     </row>
     <row r="361" spans="1:23">
+      <c r="A361" t="s">
+        <v>689</v>
+      </c>
       <c r="B361" t="s">
         <v>391</v>
       </c>
@@ -21651,6 +22530,9 @@
       </c>
     </row>
     <row r="362" spans="1:23">
+      <c r="A362" t="s">
+        <v>689</v>
+      </c>
       <c r="B362" t="s">
         <v>391</v>
       </c>
@@ -21719,6 +22601,9 @@
       </c>
     </row>
     <row r="363" spans="1:23">
+      <c r="A363" t="s">
+        <v>689</v>
+      </c>
       <c r="B363" t="s">
         <v>391</v>
       </c>
@@ -21787,6 +22672,9 @@
       </c>
     </row>
     <row r="364" spans="1:23">
+      <c r="A364" t="s">
+        <v>689</v>
+      </c>
       <c r="B364" t="s">
         <v>391</v>
       </c>
@@ -21855,6 +22743,9 @@
       </c>
     </row>
     <row r="365" spans="1:23">
+      <c r="A365" t="s">
+        <v>689</v>
+      </c>
       <c r="B365" t="s">
         <v>391</v>
       </c>
@@ -21923,6 +22814,9 @@
       </c>
     </row>
     <row r="366" spans="1:23">
+      <c r="A366" t="s">
+        <v>689</v>
+      </c>
       <c r="B366" t="s">
         <v>391</v>
       </c>
@@ -22043,7 +22937,10 @@
         <v>411</v>
       </c>
     </row>
-    <row r="369" spans="2:16">
+    <row r="369" spans="1:16">
+      <c r="A369" t="s">
+        <v>689</v>
+      </c>
       <c r="B369" t="s">
         <v>407</v>
       </c>
@@ -22090,7 +22987,10 @@
         <v>633</v>
       </c>
     </row>
-    <row r="370" spans="2:16">
+    <row r="370" spans="1:16">
+      <c r="A370" t="s">
+        <v>689</v>
+      </c>
       <c r="B370" t="s">
         <v>407</v>
       </c>
@@ -22137,7 +23037,10 @@
         <v>634</v>
       </c>
     </row>
-    <row r="371" spans="2:16">
+    <row r="371" spans="1:16">
+      <c r="A371" t="s">
+        <v>689</v>
+      </c>
       <c r="B371" t="s">
         <v>407</v>
       </c>
@@ -22184,7 +23087,10 @@
         <v>411</v>
       </c>
     </row>
-    <row r="372" spans="2:16">
+    <row r="372" spans="1:16">
+      <c r="A372" t="s">
+        <v>689</v>
+      </c>
       <c r="B372" t="s">
         <v>407</v>
       </c>
@@ -22231,7 +23137,10 @@
         <v>635</v>
       </c>
     </row>
-    <row r="373" spans="2:16">
+    <row r="373" spans="1:16">
+      <c r="A373" t="s">
+        <v>689</v>
+      </c>
       <c r="B373" t="s">
         <v>407</v>
       </c>
@@ -22278,7 +23187,10 @@
         <v>634</v>
       </c>
     </row>
-    <row r="374" spans="2:16">
+    <row r="374" spans="1:16">
+      <c r="A374" t="s">
+        <v>689</v>
+      </c>
       <c r="B374" t="s">
         <v>407</v>
       </c>
@@ -22325,7 +23237,10 @@
         <v>411</v>
       </c>
     </row>
-    <row r="375" spans="2:16">
+    <row r="375" spans="1:16">
+      <c r="A375" t="s">
+        <v>689</v>
+      </c>
       <c r="B375" t="s">
         <v>407</v>
       </c>
@@ -22372,7 +23287,10 @@
         <v>633</v>
       </c>
     </row>
-    <row r="376" spans="2:16">
+    <row r="376" spans="1:16">
+      <c r="A376" t="s">
+        <v>689</v>
+      </c>
       <c r="B376" t="s">
         <v>407</v>
       </c>
@@ -22419,7 +23337,10 @@
         <v>634</v>
       </c>
     </row>
-    <row r="377" spans="2:16">
+    <row r="377" spans="1:16">
+      <c r="A377" t="s">
+        <v>689</v>
+      </c>
       <c r="B377" t="s">
         <v>407</v>
       </c>
@@ -22466,7 +23387,10 @@
         <v>411</v>
       </c>
     </row>
-    <row r="378" spans="2:16">
+    <row r="378" spans="1:16">
+      <c r="A378" t="s">
+        <v>689</v>
+      </c>
       <c r="B378" t="s">
         <v>407</v>
       </c>
@@ -22513,7 +23437,10 @@
         <v>412</v>
       </c>
     </row>
-    <row r="379" spans="2:16">
+    <row r="379" spans="1:16">
+      <c r="A379" t="s">
+        <v>689</v>
+      </c>
       <c r="B379" t="s">
         <v>407</v>
       </c>
@@ -22560,7 +23487,10 @@
         <v>411</v>
       </c>
     </row>
-    <row r="380" spans="2:16">
+    <row r="380" spans="1:16">
+      <c r="A380" t="s">
+        <v>689</v>
+      </c>
       <c r="B380" t="s">
         <v>407</v>
       </c>
@@ -22607,7 +23537,10 @@
         <v>633</v>
       </c>
     </row>
-    <row r="381" spans="2:16">
+    <row r="381" spans="1:16">
+      <c r="A381" t="s">
+        <v>689</v>
+      </c>
       <c r="B381" t="s">
         <v>407</v>
       </c>
@@ -22654,7 +23587,10 @@
         <v>634</v>
       </c>
     </row>
-    <row r="382" spans="2:16">
+    <row r="382" spans="1:16">
+      <c r="A382" t="s">
+        <v>689</v>
+      </c>
       <c r="B382" t="s">
         <v>407</v>
       </c>
@@ -22701,7 +23637,10 @@
         <v>411</v>
       </c>
     </row>
-    <row r="383" spans="2:16">
+    <row r="383" spans="1:16">
+      <c r="A383" t="s">
+        <v>689</v>
+      </c>
       <c r="B383" t="s">
         <v>407</v>
       </c>
@@ -22748,7 +23687,10 @@
         <v>633</v>
       </c>
     </row>
-    <row r="384" spans="2:16">
+    <row r="384" spans="1:16">
+      <c r="A384" t="s">
+        <v>689</v>
+      </c>
       <c r="B384" t="s">
         <v>407</v>
       </c>
@@ -22795,7 +23737,10 @@
         <v>634</v>
       </c>
     </row>
-    <row r="385" spans="2:16">
+    <row r="385" spans="1:16">
+      <c r="A385" t="s">
+        <v>689</v>
+      </c>
       <c r="B385" t="s">
         <v>407</v>
       </c>
@@ -22842,7 +23787,10 @@
         <v>411</v>
       </c>
     </row>
-    <row r="386" spans="2:16">
+    <row r="386" spans="1:16">
+      <c r="A386" t="s">
+        <v>689</v>
+      </c>
       <c r="B386" t="s">
         <v>407</v>
       </c>
@@ -22889,7 +23837,10 @@
         <v>633</v>
       </c>
     </row>
-    <row r="387" spans="2:16">
+    <row r="387" spans="1:16">
+      <c r="A387" t="s">
+        <v>689</v>
+      </c>
       <c r="B387" t="s">
         <v>407</v>
       </c>
@@ -22936,7 +23887,10 @@
         <v>634</v>
       </c>
     </row>
-    <row r="388" spans="2:16">
+    <row r="388" spans="1:16">
+      <c r="A388" t="s">
+        <v>689</v>
+      </c>
       <c r="B388" t="s">
         <v>407</v>
       </c>
@@ -22983,7 +23937,10 @@
         <v>411</v>
       </c>
     </row>
-    <row r="389" spans="2:16">
+    <row r="389" spans="1:16">
+      <c r="A389" t="s">
+        <v>689</v>
+      </c>
       <c r="B389" t="s">
         <v>407</v>
       </c>
@@ -23030,7 +23987,10 @@
         <v>633</v>
       </c>
     </row>
-    <row r="390" spans="2:16">
+    <row r="390" spans="1:16">
+      <c r="A390" t="s">
+        <v>689</v>
+      </c>
       <c r="B390" t="s">
         <v>407</v>
       </c>
@@ -23077,7 +24037,10 @@
         <v>634</v>
       </c>
     </row>
-    <row r="391" spans="2:16">
+    <row r="391" spans="1:16">
+      <c r="A391" t="s">
+        <v>689</v>
+      </c>
       <c r="B391" t="s">
         <v>407</v>
       </c>
@@ -23124,7 +24087,10 @@
         <v>411</v>
       </c>
     </row>
-    <row r="392" spans="2:16">
+    <row r="392" spans="1:16">
+      <c r="A392" t="s">
+        <v>689</v>
+      </c>
       <c r="B392" t="s">
         <v>407</v>
       </c>
@@ -23171,7 +24137,10 @@
         <v>633</v>
       </c>
     </row>
-    <row r="393" spans="2:16">
+    <row r="393" spans="1:16">
+      <c r="A393" t="s">
+        <v>689</v>
+      </c>
       <c r="B393" t="s">
         <v>407</v>
       </c>
@@ -23218,7 +24187,10 @@
         <v>634</v>
       </c>
     </row>
-    <row r="394" spans="2:16">
+    <row r="394" spans="1:16">
+      <c r="A394" t="s">
+        <v>689</v>
+      </c>
       <c r="B394" t="s">
         <v>407</v>
       </c>
@@ -23265,7 +24237,10 @@
         <v>411</v>
       </c>
     </row>
-    <row r="395" spans="2:16">
+    <row r="395" spans="1:16">
+      <c r="A395" t="s">
+        <v>689</v>
+      </c>
       <c r="B395" t="s">
         <v>407</v>
       </c>
@@ -23312,7 +24287,10 @@
         <v>412</v>
       </c>
     </row>
-    <row r="396" spans="2:16">
+    <row r="396" spans="1:16">
+      <c r="A396" t="s">
+        <v>689</v>
+      </c>
       <c r="B396" t="s">
         <v>407</v>
       </c>
@@ -23359,7 +24337,10 @@
         <v>411</v>
       </c>
     </row>
-    <row r="397" spans="2:16">
+    <row r="397" spans="1:16">
+      <c r="A397" t="s">
+        <v>689</v>
+      </c>
       <c r="B397" t="s">
         <v>407</v>
       </c>
@@ -23406,7 +24387,10 @@
         <v>633</v>
       </c>
     </row>
-    <row r="398" spans="2:16">
+    <row r="398" spans="1:16">
+      <c r="A398" t="s">
+        <v>689</v>
+      </c>
       <c r="B398" t="s">
         <v>407</v>
       </c>
@@ -23453,7 +24437,10 @@
         <v>634</v>
       </c>
     </row>
-    <row r="399" spans="2:16">
+    <row r="399" spans="1:16">
+      <c r="A399" t="s">
+        <v>689</v>
+      </c>
       <c r="B399" t="s">
         <v>407</v>
       </c>
@@ -23500,7 +24487,10 @@
         <v>411</v>
       </c>
     </row>
-    <row r="400" spans="2:16">
+    <row r="400" spans="1:16">
+      <c r="A400" t="s">
+        <v>689</v>
+      </c>
       <c r="B400" t="s">
         <v>407</v>
       </c>
@@ -23548,6 +24538,9 @@
       </c>
     </row>
     <row r="401" spans="1:16">
+      <c r="A401" t="s">
+        <v>689</v>
+      </c>
       <c r="B401" t="s">
         <v>407</v>
       </c>
@@ -23595,6 +24588,9 @@
       </c>
     </row>
     <row r="402" spans="1:16">
+      <c r="A402" t="s">
+        <v>689</v>
+      </c>
       <c r="B402" t="s">
         <v>407</v>
       </c>
@@ -23642,6 +24638,9 @@
       </c>
     </row>
     <row r="403" spans="1:16">
+      <c r="A403" t="s">
+        <v>689</v>
+      </c>
       <c r="B403" t="s">
         <v>407</v>
       </c>
@@ -23689,6 +24688,9 @@
       </c>
     </row>
     <row r="404" spans="1:16">
+      <c r="A404" t="s">
+        <v>689</v>
+      </c>
       <c r="B404" t="s">
         <v>407</v>
       </c>
@@ -23736,6 +24738,9 @@
       </c>
     </row>
     <row r="405" spans="1:16">
+      <c r="A405" t="s">
+        <v>689</v>
+      </c>
       <c r="B405" t="s">
         <v>407</v>
       </c>
@@ -23783,6 +24788,9 @@
       </c>
     </row>
     <row r="406" spans="1:16">
+      <c r="A406" t="s">
+        <v>689</v>
+      </c>
       <c r="B406" t="s">
         <v>407</v>
       </c>
@@ -23830,6 +24838,9 @@
       </c>
     </row>
     <row r="407" spans="1:16">
+      <c r="A407" t="s">
+        <v>689</v>
+      </c>
       <c r="B407" t="s">
         <v>407</v>
       </c>
@@ -23927,6 +24938,9 @@
       </c>
     </row>
     <row r="410" spans="1:16">
+      <c r="A410" t="s">
+        <v>689</v>
+      </c>
       <c r="B410" t="s">
         <v>440</v>
       </c>
@@ -23974,6 +24988,9 @@
       </c>
     </row>
     <row r="411" spans="1:16">
+      <c r="A411" t="s">
+        <v>689</v>
+      </c>
       <c r="B411" t="s">
         <v>440</v>
       </c>
@@ -24021,6 +25038,9 @@
       </c>
     </row>
     <row r="412" spans="1:16">
+      <c r="A412" t="s">
+        <v>689</v>
+      </c>
       <c r="B412" t="s">
         <v>440</v>
       </c>
@@ -24068,6 +25088,9 @@
       </c>
     </row>
     <row r="413" spans="1:16">
+      <c r="A413" t="s">
+        <v>689</v>
+      </c>
       <c r="B413" t="s">
         <v>440</v>
       </c>
@@ -24115,6 +25138,9 @@
       </c>
     </row>
     <row r="414" spans="1:16">
+      <c r="A414" t="s">
+        <v>689</v>
+      </c>
       <c r="B414" t="s">
         <v>440</v>
       </c>
@@ -24162,6 +25188,9 @@
       </c>
     </row>
     <row r="415" spans="1:16">
+      <c r="A415" t="s">
+        <v>689</v>
+      </c>
       <c r="B415" t="s">
         <v>440</v>
       </c>
@@ -24209,6 +25238,9 @@
       </c>
     </row>
     <row r="416" spans="1:16">
+      <c r="A416" t="s">
+        <v>689</v>
+      </c>
       <c r="B416" t="s">
         <v>440</v>
       </c>
@@ -24255,7 +25287,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="417" spans="2:16">
+    <row r="417" spans="1:16">
+      <c r="A417" t="s">
+        <v>689</v>
+      </c>
       <c r="B417" t="s">
         <v>440</v>
       </c>
@@ -24302,7 +25337,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="418" spans="2:16">
+    <row r="418" spans="1:16">
+      <c r="A418" t="s">
+        <v>689</v>
+      </c>
       <c r="B418" t="s">
         <v>440</v>
       </c>
@@ -24349,7 +25387,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="419" spans="2:16">
+    <row r="419" spans="1:16">
+      <c r="A419" t="s">
+        <v>689</v>
+      </c>
       <c r="B419" t="s">
         <v>440</v>
       </c>
@@ -24396,7 +25437,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="420" spans="2:16">
+    <row r="420" spans="1:16">
+      <c r="A420" t="s">
+        <v>689</v>
+      </c>
       <c r="B420" t="s">
         <v>440</v>
       </c>
@@ -24443,7 +25487,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="421" spans="2:16">
+    <row r="421" spans="1:16">
+      <c r="A421" t="s">
+        <v>689</v>
+      </c>
       <c r="B421" t="s">
         <v>440</v>
       </c>
@@ -24490,7 +25537,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="422" spans="2:16">
+    <row r="422" spans="1:16">
+      <c r="A422" t="s">
+        <v>689</v>
+      </c>
       <c r="B422" t="s">
         <v>440</v>
       </c>
@@ -24537,7 +25587,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="423" spans="2:16">
+    <row r="423" spans="1:16">
+      <c r="A423" t="s">
+        <v>689</v>
+      </c>
       <c r="B423" t="s">
         <v>440</v>
       </c>
@@ -24584,7 +25637,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="424" spans="2:16">
+    <row r="424" spans="1:16">
+      <c r="A424" t="s">
+        <v>689</v>
+      </c>
       <c r="B424" t="s">
         <v>440</v>
       </c>
@@ -24631,7 +25687,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="425" spans="2:16">
+    <row r="425" spans="1:16">
+      <c r="A425" t="s">
+        <v>689</v>
+      </c>
       <c r="B425" t="s">
         <v>440</v>
       </c>
@@ -24678,7 +25737,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="426" spans="2:16">
+    <row r="426" spans="1:16">
+      <c r="A426" t="s">
+        <v>689</v>
+      </c>
       <c r="B426" t="s">
         <v>440</v>
       </c>
@@ -24725,7 +25787,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="427" spans="2:16">
+    <row r="427" spans="1:16">
+      <c r="A427" t="s">
+        <v>689</v>
+      </c>
       <c r="B427" t="s">
         <v>440</v>
       </c>
@@ -24772,7 +25837,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="428" spans="2:16">
+    <row r="428" spans="1:16">
+      <c r="A428" t="s">
+        <v>689</v>
+      </c>
       <c r="B428" t="s">
         <v>440</v>
       </c>
@@ -24819,7 +25887,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="429" spans="2:16">
+    <row r="429" spans="1:16">
+      <c r="A429" t="s">
+        <v>689</v>
+      </c>
       <c r="B429" t="s">
         <v>440</v>
       </c>
@@ -24866,7 +25937,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="430" spans="2:16">
+    <row r="430" spans="1:16">
+      <c r="A430" t="s">
+        <v>689</v>
+      </c>
       <c r="B430" t="s">
         <v>440</v>
       </c>
@@ -24913,7 +25987,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="431" spans="2:16">
+    <row r="431" spans="1:16">
+      <c r="A431" t="s">
+        <v>689</v>
+      </c>
       <c r="B431" t="s">
         <v>440</v>
       </c>
@@ -24960,7 +26037,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="432" spans="2:16">
+    <row r="432" spans="1:16">
+      <c r="A432" t="s">
+        <v>689</v>
+      </c>
       <c r="B432" t="s">
         <v>440</v>
       </c>
@@ -25008,6 +26088,9 @@
       </c>
     </row>
     <row r="433" spans="1:16">
+      <c r="A433" t="s">
+        <v>689</v>
+      </c>
       <c r="B433" t="s">
         <v>440</v>
       </c>
@@ -25055,6 +26138,9 @@
       </c>
     </row>
     <row r="434" spans="1:16">
+      <c r="A434" t="s">
+        <v>689</v>
+      </c>
       <c r="B434" t="s">
         <v>440</v>
       </c>
@@ -25152,6 +26238,9 @@
       </c>
     </row>
     <row r="437" spans="1:16">
+      <c r="A437" t="s">
+        <v>689</v>
+      </c>
       <c r="B437" t="s">
         <v>498</v>
       </c>
@@ -25199,6 +26288,9 @@
       </c>
     </row>
     <row r="438" spans="1:16">
+      <c r="A438" t="s">
+        <v>689</v>
+      </c>
       <c r="B438" t="s">
         <v>498</v>
       </c>
@@ -25246,6 +26338,9 @@
       </c>
     </row>
     <row r="439" spans="1:16">
+      <c r="A439" t="s">
+        <v>689</v>
+      </c>
       <c r="B439" t="s">
         <v>498</v>
       </c>
@@ -25293,6 +26388,9 @@
       </c>
     </row>
     <row r="440" spans="1:16">
+      <c r="A440" t="s">
+        <v>689</v>
+      </c>
       <c r="B440" t="s">
         <v>498</v>
       </c>
@@ -25340,6 +26438,9 @@
       </c>
     </row>
     <row r="441" spans="1:16">
+      <c r="A441" t="s">
+        <v>689</v>
+      </c>
       <c r="B441" t="s">
         <v>498</v>
       </c>
@@ -25387,6 +26488,9 @@
       </c>
     </row>
     <row r="442" spans="1:16">
+      <c r="A442" t="s">
+        <v>689</v>
+      </c>
       <c r="B442" t="s">
         <v>498</v>
       </c>
@@ -25434,6 +26538,9 @@
       </c>
     </row>
     <row r="443" spans="1:16">
+      <c r="A443" t="s">
+        <v>689</v>
+      </c>
       <c r="B443" t="s">
         <v>498</v>
       </c>
@@ -25481,6 +26588,9 @@
       </c>
     </row>
     <row r="444" spans="1:16">
+      <c r="A444" t="s">
+        <v>689</v>
+      </c>
       <c r="B444" t="s">
         <v>498</v>
       </c>
@@ -25528,6 +26638,9 @@
       </c>
     </row>
     <row r="445" spans="1:16">
+      <c r="A445" t="s">
+        <v>689</v>
+      </c>
       <c r="B445" t="s">
         <v>498</v>
       </c>
@@ -25575,6 +26688,9 @@
       </c>
     </row>
     <row r="446" spans="1:16">
+      <c r="A446" t="s">
+        <v>689</v>
+      </c>
       <c r="B446" t="s">
         <v>498</v>
       </c>
@@ -25622,6 +26738,9 @@
       </c>
     </row>
     <row r="447" spans="1:16">
+      <c r="A447" t="s">
+        <v>689</v>
+      </c>
       <c r="B447" t="s">
         <v>498</v>
       </c>
@@ -25669,6 +26788,9 @@
       </c>
     </row>
     <row r="448" spans="1:16">
+      <c r="A448" t="s">
+        <v>689</v>
+      </c>
       <c r="B448" t="s">
         <v>498</v>
       </c>
@@ -25716,6 +26838,9 @@
       </c>
     </row>
     <row r="449" spans="1:23">
+      <c r="A449" t="s">
+        <v>689</v>
+      </c>
       <c r="B449" t="s">
         <v>498</v>
       </c>
@@ -25763,6 +26888,9 @@
       </c>
     </row>
     <row r="450" spans="1:23">
+      <c r="A450" t="s">
+        <v>689</v>
+      </c>
       <c r="B450" t="s">
         <v>498</v>
       </c>
@@ -25810,6 +26938,9 @@
       </c>
     </row>
     <row r="451" spans="1:23">
+      <c r="A451" t="s">
+        <v>689</v>
+      </c>
       <c r="B451" t="s">
         <v>498</v>
       </c>
@@ -25931,6 +27062,9 @@
       </c>
     </row>
     <row r="454" spans="1:23">
+      <c r="A454" t="s">
+        <v>689</v>
+      </c>
       <c r="B454" t="s">
         <v>446</v>
       </c>
@@ -25999,6 +27133,9 @@
       </c>
     </row>
     <row r="455" spans="1:23">
+      <c r="A455" t="s">
+        <v>689</v>
+      </c>
       <c r="B455" t="s">
         <v>446</v>
       </c>
@@ -26067,6 +27204,9 @@
       </c>
     </row>
     <row r="456" spans="1:23">
+      <c r="A456" t="s">
+        <v>689</v>
+      </c>
       <c r="B456" t="s">
         <v>446</v>
       </c>
@@ -26135,6 +27275,9 @@
       </c>
     </row>
     <row r="457" spans="1:23">
+      <c r="A457" t="s">
+        <v>689</v>
+      </c>
       <c r="B457" t="s">
         <v>446</v>
       </c>
@@ -26203,6 +27346,9 @@
       </c>
     </row>
     <row r="458" spans="1:23">
+      <c r="A458" t="s">
+        <v>689</v>
+      </c>
       <c r="B458" t="s">
         <v>446</v>
       </c>
@@ -26271,6 +27417,9 @@
       </c>
     </row>
     <row r="459" spans="1:23">
+      <c r="A459" t="s">
+        <v>689</v>
+      </c>
       <c r="B459" t="s">
         <v>446</v>
       </c>
@@ -26339,6 +27488,9 @@
       </c>
     </row>
     <row r="460" spans="1:23">
+      <c r="A460" t="s">
+        <v>689</v>
+      </c>
       <c r="B460" t="s">
         <v>446</v>
       </c>
@@ -26407,6 +27559,9 @@
       </c>
     </row>
     <row r="461" spans="1:23">
+      <c r="A461" t="s">
+        <v>689</v>
+      </c>
       <c r="B461" t="s">
         <v>446</v>
       </c>
@@ -26475,6 +27630,9 @@
       </c>
     </row>
     <row r="462" spans="1:23">
+      <c r="A462" t="s">
+        <v>689</v>
+      </c>
       <c r="B462" t="s">
         <v>446</v>
       </c>
@@ -26543,6 +27701,9 @@
       </c>
     </row>
     <row r="463" spans="1:23">
+      <c r="A463" t="s">
+        <v>689</v>
+      </c>
       <c r="B463" t="s">
         <v>446</v>
       </c>
@@ -26611,6 +27772,9 @@
       </c>
     </row>
     <row r="464" spans="1:23">
+      <c r="A464" t="s">
+        <v>689</v>
+      </c>
       <c r="B464" t="s">
         <v>446</v>
       </c>
@@ -26678,7 +27842,10 @@
         <v>674</v>
       </c>
     </row>
-    <row r="465" spans="2:23">
+    <row r="465" spans="1:23">
+      <c r="A465" t="s">
+        <v>689</v>
+      </c>
       <c r="B465" t="s">
         <v>446</v>
       </c>
@@ -26746,7 +27913,10 @@
         <v>674</v>
       </c>
     </row>
-    <row r="466" spans="2:23">
+    <row r="466" spans="1:23">
+      <c r="A466" t="s">
+        <v>689</v>
+      </c>
       <c r="B466" t="s">
         <v>446</v>
       </c>
@@ -26814,7 +27984,10 @@
         <v>674</v>
       </c>
     </row>
-    <row r="467" spans="2:23">
+    <row r="467" spans="1:23">
+      <c r="A467" t="s">
+        <v>689</v>
+      </c>
       <c r="B467" t="s">
         <v>446</v>
       </c>
@@ -26882,7 +28055,10 @@
         <v>674</v>
       </c>
     </row>
-    <row r="468" spans="2:23">
+    <row r="468" spans="1:23">
+      <c r="A468" t="s">
+        <v>689</v>
+      </c>
       <c r="B468" t="s">
         <v>446</v>
       </c>
@@ -26950,7 +28126,10 @@
         <v>674</v>
       </c>
     </row>
-    <row r="469" spans="2:23">
+    <row r="469" spans="1:23">
+      <c r="A469" t="s">
+        <v>689</v>
+      </c>
       <c r="B469" t="s">
         <v>446</v>
       </c>
@@ -27018,7 +28197,10 @@
         <v>674</v>
       </c>
     </row>
-    <row r="470" spans="2:23">
+    <row r="470" spans="1:23">
+      <c r="A470" t="s">
+        <v>689</v>
+      </c>
       <c r="B470" t="s">
         <v>446</v>
       </c>
@@ -27086,7 +28268,10 @@
         <v>674</v>
       </c>
     </row>
-    <row r="471" spans="2:23">
+    <row r="471" spans="1:23">
+      <c r="A471" t="s">
+        <v>689</v>
+      </c>
       <c r="B471" t="s">
         <v>446</v>
       </c>
@@ -27154,7 +28339,10 @@
         <v>674</v>
       </c>
     </row>
-    <row r="472" spans="2:23">
+    <row r="472" spans="1:23">
+      <c r="A472" t="s">
+        <v>689</v>
+      </c>
       <c r="B472" t="s">
         <v>446</v>
       </c>
@@ -27222,7 +28410,10 @@
         <v>674</v>
       </c>
     </row>
-    <row r="473" spans="2:23">
+    <row r="473" spans="1:23">
+      <c r="A473" t="s">
+        <v>689</v>
+      </c>
       <c r="B473" t="s">
         <v>446</v>
       </c>
@@ -27290,7 +28481,10 @@
         <v>674</v>
       </c>
     </row>
-    <row r="474" spans="2:23">
+    <row r="474" spans="1:23">
+      <c r="A474" t="s">
+        <v>689</v>
+      </c>
       <c r="B474" t="s">
         <v>446</v>
       </c>
@@ -27358,7 +28552,10 @@
         <v>674</v>
       </c>
     </row>
-    <row r="475" spans="2:23">
+    <row r="475" spans="1:23">
+      <c r="A475" t="s">
+        <v>689</v>
+      </c>
       <c r="B475" t="s">
         <v>446</v>
       </c>
@@ -27426,7 +28623,10 @@
         <v>674</v>
       </c>
     </row>
-    <row r="476" spans="2:23">
+    <row r="476" spans="1:23">
+      <c r="A476" t="s">
+        <v>689</v>
+      </c>
       <c r="B476" t="s">
         <v>446</v>
       </c>
@@ -27494,7 +28694,10 @@
         <v>674</v>
       </c>
     </row>
-    <row r="477" spans="2:23">
+    <row r="477" spans="1:23">
+      <c r="A477" t="s">
+        <v>689</v>
+      </c>
       <c r="B477" t="s">
         <v>446</v>
       </c>
@@ -27562,7 +28765,10 @@
         <v>674</v>
       </c>
     </row>
-    <row r="478" spans="2:23">
+    <row r="478" spans="1:23">
+      <c r="A478" t="s">
+        <v>689</v>
+      </c>
       <c r="B478" t="s">
         <v>446</v>
       </c>
@@ -27630,7 +28836,10 @@
         <v>674</v>
       </c>
     </row>
-    <row r="479" spans="2:23">
+    <row r="479" spans="1:23">
+      <c r="A479" t="s">
+        <v>689</v>
+      </c>
       <c r="B479" t="s">
         <v>446</v>
       </c>
@@ -27698,7 +28907,10 @@
         <v>674</v>
       </c>
     </row>
-    <row r="480" spans="2:23">
+    <row r="480" spans="1:23">
+      <c r="A480" t="s">
+        <v>689</v>
+      </c>
       <c r="B480" t="s">
         <v>446</v>
       </c>
@@ -27767,6 +28979,9 @@
       </c>
     </row>
     <row r="481" spans="1:23">
+      <c r="A481" t="s">
+        <v>689</v>
+      </c>
       <c r="B481" t="s">
         <v>446</v>
       </c>
@@ -27835,6 +29050,9 @@
       </c>
     </row>
     <row r="482" spans="1:23">
+      <c r="A482" t="s">
+        <v>689</v>
+      </c>
       <c r="B482" t="s">
         <v>446</v>
       </c>
@@ -27956,6 +29174,9 @@
       </c>
     </row>
     <row r="485" spans="1:23">
+      <c r="A485" t="s">
+        <v>689</v>
+      </c>
       <c r="B485" t="s">
         <v>500</v>
       </c>
@@ -28003,6 +29224,9 @@
       </c>
     </row>
     <row r="486" spans="1:23">
+      <c r="A486" t="s">
+        <v>689</v>
+      </c>
       <c r="B486" t="s">
         <v>500</v>
       </c>
@@ -28050,6 +29274,9 @@
       </c>
     </row>
     <row r="487" spans="1:23">
+      <c r="A487" t="s">
+        <v>689</v>
+      </c>
       <c r="B487" t="s">
         <v>500</v>
       </c>
@@ -28097,6 +29324,9 @@
       </c>
     </row>
     <row r="488" spans="1:23">
+      <c r="A488" t="s">
+        <v>689</v>
+      </c>
       <c r="B488" t="s">
         <v>500</v>
       </c>
@@ -28144,6 +29374,9 @@
       </c>
     </row>
     <row r="489" spans="1:23">
+      <c r="A489" t="s">
+        <v>689</v>
+      </c>
       <c r="B489" t="s">
         <v>500</v>
       </c>
@@ -28191,6 +29424,9 @@
       </c>
     </row>
     <row r="490" spans="1:23">
+      <c r="A490" t="s">
+        <v>689</v>
+      </c>
       <c r="B490" t="s">
         <v>500</v>
       </c>
@@ -28238,6 +29474,9 @@
       </c>
     </row>
     <row r="491" spans="1:23">
+      <c r="A491" t="s">
+        <v>689</v>
+      </c>
       <c r="B491" t="s">
         <v>500</v>
       </c>
@@ -28285,6 +29524,9 @@
       </c>
     </row>
     <row r="492" spans="1:23">
+      <c r="A492" t="s">
+        <v>689</v>
+      </c>
       <c r="B492" t="s">
         <v>500</v>
       </c>
@@ -28333,7 +29575,7 @@
     </row>
     <row r="494" spans="1:23">
       <c r="A494" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B494" t="s">
         <v>472</v>
@@ -28382,6 +29624,9 @@
       </c>
     </row>
     <row r="495" spans="1:23">
+      <c r="A495" t="s">
+        <v>688</v>
+      </c>
       <c r="B495" t="s">
         <v>472</v>
       </c>
@@ -28429,6 +29674,9 @@
       </c>
     </row>
     <row r="496" spans="1:23">
+      <c r="A496" t="s">
+        <v>688</v>
+      </c>
       <c r="B496" t="s">
         <v>472</v>
       </c>
@@ -28475,7 +29723,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="497" spans="2:16">
+    <row r="497" spans="1:16">
+      <c r="A497" t="s">
+        <v>688</v>
+      </c>
       <c r="B497" t="s">
         <v>472</v>
       </c>
@@ -28522,7 +29773,10 @@
         <v>568</v>
       </c>
     </row>
-    <row r="498" spans="2:16">
+    <row r="498" spans="1:16">
+      <c r="A498" t="s">
+        <v>688</v>
+      </c>
       <c r="B498" t="s">
         <v>472</v>
       </c>
@@ -28569,7 +29823,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="499" spans="2:16">
+    <row r="499" spans="1:16">
+      <c r="A499" t="s">
+        <v>688</v>
+      </c>
       <c r="B499" t="s">
         <v>472</v>
       </c>
@@ -28616,7 +29873,10 @@
         <v>568</v>
       </c>
     </row>
-    <row r="500" spans="2:16">
+    <row r="500" spans="1:16">
+      <c r="A500" t="s">
+        <v>688</v>
+      </c>
       <c r="B500" t="s">
         <v>472</v>
       </c>
@@ -28663,7 +29923,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="501" spans="2:16">
+    <row r="501" spans="1:16">
+      <c r="A501" t="s">
+        <v>688</v>
+      </c>
       <c r="B501" t="s">
         <v>472</v>
       </c>
@@ -28710,7 +29973,10 @@
         <v>568</v>
       </c>
     </row>
-    <row r="502" spans="2:16">
+    <row r="502" spans="1:16">
+      <c r="A502" t="s">
+        <v>688</v>
+      </c>
       <c r="B502" t="s">
         <v>472</v>
       </c>
@@ -28757,7 +30023,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="503" spans="2:16">
+    <row r="503" spans="1:16">
+      <c r="A503" t="s">
+        <v>688</v>
+      </c>
       <c r="B503" t="s">
         <v>472</v>
       </c>
@@ -28804,7 +30073,10 @@
         <v>568</v>
       </c>
     </row>
-    <row r="504" spans="2:16">
+    <row r="504" spans="1:16">
+      <c r="A504" t="s">
+        <v>688</v>
+      </c>
       <c r="B504" t="s">
         <v>472</v>
       </c>
@@ -28851,7 +30123,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="505" spans="2:16">
+    <row r="505" spans="1:16">
+      <c r="A505" t="s">
+        <v>688</v>
+      </c>
       <c r="B505" t="s">
         <v>472</v>
       </c>
@@ -28898,7 +30173,10 @@
         <v>568</v>
       </c>
     </row>
-    <row r="506" spans="2:16">
+    <row r="506" spans="1:16">
+      <c r="A506" t="s">
+        <v>688</v>
+      </c>
       <c r="B506" t="s">
         <v>472</v>
       </c>
@@ -28945,7 +30223,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="507" spans="2:16">
+    <row r="507" spans="1:16">
+      <c r="A507" t="s">
+        <v>688</v>
+      </c>
       <c r="B507" t="s">
         <v>472</v>
       </c>

</xml_diff>